<commit_message>
added packaging to write excel
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1,13 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
   <si>
     <t>Šifra</t>
   </si>
@@ -65,12 +64,12 @@
     <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus</t>
   </si>
   <si>
+    <t>Kvasovke in plesni</t>
+  </si>
+  <si>
     <t>Enterobakterije</t>
   </si>
   <si>
-    <t>Kvasovke in plesni</t>
-  </si>
-  <si>
     <t>Gostota</t>
   </si>
   <si>
@@ -101,13 +100,106 @@
     <t>Sladkorji</t>
   </si>
   <si>
+    <t>Beljakovine</t>
+  </si>
+  <si>
+    <t>Sol</t>
+  </si>
+  <si>
     <t>Prehranske vlaknine</t>
   </si>
   <si>
-    <t>Beljakovine</t>
-  </si>
-  <si>
-    <t>Sol</t>
+    <t>neto</t>
+  </si>
+  <si>
+    <t>tip MPE</t>
+  </si>
+  <si>
+    <t>tip TP</t>
+  </si>
+  <si>
+    <t>dimenzija MPE</t>
+  </si>
+  <si>
+    <t>dimenzija TP</t>
+  </si>
+  <si>
+    <t>tip KP</t>
+  </si>
+  <si>
+    <t>število MPE</t>
+  </si>
+  <si>
+    <t>dimenzija KP</t>
+  </si>
+  <si>
+    <t>število plasti na paleti</t>
+  </si>
+  <si>
+    <t>rok uporabe</t>
+  </si>
+  <si>
+    <t>embalaža</t>
+  </si>
+  <si>
+    <t>način skladiščenja in transporta</t>
+  </si>
+  <si>
+    <t>32226</t>
+  </si>
+  <si>
+    <t>GUARANA NATURAL ENERGY 5 X 9 ml</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Naravni kofein iz gvarane in niacin v raztopini</t>
+  </si>
+  <si>
+    <t>Voda, trsni sladkor, 10 % izvleček iz semen gvarane v prahu (Paulina cupana), zgoščeni sok aronije, zgoščeni sok borovnice, uprašeni sok acerole (Malpighia glabra), niacin in konzervans: kalijev sorbat.</t>
+  </si>
+  <si>
+    <t>Temno vijolična tekočina z usedlino na dnu fiole, brez tujih primesi</t>
+  </si>
+  <si>
+    <t>Grenko sladkega okusa, aroma po borovnici in gvarani</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z veljavno evropsko in nacionalno zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP.</t>
+  </si>
+  <si>
+    <t>&lt;10 CFU/g</t>
+  </si>
+  <si>
+    <t>&lt;500 CFU/g</t>
+  </si>
+  <si>
+    <t>neg./25 g</t>
+  </si>
+  <si>
+    <t>&lt;1.000 CFU/ g</t>
+  </si>
+  <si>
+    <t>1,1660 g/ml (1,1427 – 1,1893) g/ml</t>
+  </si>
+  <si>
+    <t>45 ml (5 x 9 ml)</t>
+  </si>
+  <si>
+    <t>5 steklenih fiol s PP pokrovčki v plastičnem vložku in kartonski zloženki</t>
+  </si>
+  <si>
+    <t>127x115x24</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>24 mesecev</t>
   </si>
   <si>
     <t>32348</t>
@@ -116,9 +208,6 @@
     <t>SIRUP SMREKOVI VRŠIČKI 200 ML</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>Sirup s smrekovimi vršički, medom in vitaminoma A in C</t>
   </si>
   <si>
@@ -131,18 +220,12 @@
     <t>sladkega okusa, aroma po medu, timijanu, poprovi meti in evkaliptusu</t>
   </si>
   <si>
-    <t>Izdelek je v skladu z veljavno evropsko in nacionalno zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP.</t>
-  </si>
-  <si>
     <t>neg./0,01 g</t>
   </si>
   <si>
     <t>&lt; 100/g</t>
   </si>
   <si>
-    <t>neg./25 g</t>
-  </si>
-  <si>
     <t>neg./0,1 g</t>
   </si>
   <si>
@@ -152,34 +235,145 @@
     <t>75,0 % (74,0 – 76,0) %</t>
   </si>
   <si>
-    <t>32226</t>
-  </si>
-  <si>
-    <t>GUARANA NATURAL ENERGY 5 X 9 ml</t>
-  </si>
-  <si>
-    <t>Naravni kofein iz gvarane in niacin v raztopini</t>
-  </si>
-  <si>
-    <t>Voda, trsni sladkor, 10 % izvleček iz semen gvarane v prahu (Paulina cupana), zgoščeni sok aronije, zgoščeni sok borovnice, uprašeni sok acerole (Malpighia glabra), niacin in konzervans: kalijev sorbat.</t>
-  </si>
-  <si>
-    <t>Temno vijolična tekočina z usedlino na dnu fiole, brez tujih primesi</t>
-  </si>
-  <si>
-    <t>Grenko sladkega okusa, aroma po borovnici in gvarani</t>
-  </si>
-  <si>
-    <t>&lt;10 CFU/g</t>
-  </si>
-  <si>
-    <t>&lt;500 CFU/g</t>
-  </si>
-  <si>
-    <t>&lt;1.000 CFU/ g</t>
-  </si>
-  <si>
-    <t>1,1660 g/ml (1,1427 – 1,1893) g/ml</t>
+    <t>200 ml</t>
+  </si>
+  <si>
+    <t>temna steklenička s pokrovčkom v kartonski zloženki</t>
+  </si>
+  <si>
+    <t>6 MPE ovitih v prozorno folijo</t>
+  </si>
+  <si>
+    <t>57x57x131</t>
+  </si>
+  <si>
+    <t>195x130x150</t>
+  </si>
+  <si>
+    <t>1188</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>61001</t>
+  </si>
+  <si>
+    <t>32306</t>
+  </si>
+  <si>
+    <t>CVETNI PRAH V VREČKI 150 g</t>
+  </si>
+  <si>
+    <t>Naravni čebelji pridelek</t>
+  </si>
+  <si>
+    <t>Cvetni prah 100 %</t>
+  </si>
+  <si>
+    <t>Granule različne barve od rumene, rdeče, rjave do sive, različnih oblik in velikosti</t>
+  </si>
+  <si>
+    <t>Grenko sladkega okusa</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z nacionalno in evropsko zakonodajo Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
+  </si>
+  <si>
+    <t>&lt; 10.000/g</t>
+  </si>
+  <si>
+    <t>≤ 9,0 %</t>
+  </si>
+  <si>
+    <t>150 g</t>
+  </si>
+  <si>
+    <t>Vrečke z zip zapiranjem</t>
+  </si>
+  <si>
+    <t>55x55x105</t>
+  </si>
+  <si>
+    <t>6 MPE kartonasti zbirni zloženki</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>290x145x230</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>18 mesecev</t>
+  </si>
+  <si>
+    <t>30140</t>
+  </si>
+  <si>
+    <t>MED AKACIJEV S TARTUFI 250 G</t>
+  </si>
+  <si>
+    <t>Akacijev med s tartufi</t>
+  </si>
+  <si>
+    <t>Akacijev med 99 %, črni tartufi (Tuber aestivum) 1 %</t>
+  </si>
+  <si>
+    <t>Gosta, viskozna tekočina rumene barve, z rjavimi, črnimi koščki tartufov na vrhu kozarca</t>
+  </si>
+  <si>
+    <t>Prevladujoča, značilna za tartufe</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z veljavno nacionalno in evropsko zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
+  </si>
+  <si>
+    <t>['1429', 'kJ']</t>
+  </si>
+  <si>
+    <t>['336', 'kcal']</t>
+  </si>
+  <si>
+    <t>['0,4', 'g']</t>
+  </si>
+  <si>
+    <t>['0', 'g']</t>
+  </si>
+  <si>
+    <t>['83', 'g']</t>
+  </si>
+  <si>
+    <t>['0,2', 'g']</t>
+  </si>
+  <si>
+    <t>['0,018', 'g']</t>
+  </si>
+  <si>
+    <t>250 g</t>
+  </si>
+  <si>
+    <t>Steklen kozarec s kovinskim pokrovčkom</t>
+  </si>
+  <si>
+    <t>6 MPE v kartonskem podstavku povitih s folijo</t>
+  </si>
+  <si>
+    <t>62x65x85</t>
+  </si>
+  <si>
+    <t>192x138x87</t>
+  </si>
+  <si>
+    <t>1392</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Steklen kozarec s črnim kovinskim pokrovom</t>
   </si>
   <si>
     <t>40408</t>
@@ -218,43 +412,37 @@
     <t>['21,7', 'g']</t>
   </si>
   <si>
+    <t>['8,1', 'g']</t>
+  </si>
+  <si>
+    <t>['0,1', 'g']</t>
+  </si>
+  <si>
     <t>['7,7', 'g']</t>
   </si>
   <si>
-    <t>['8,1', 'g']</t>
-  </si>
-  <si>
-    <t>['0,1', 'g']</t>
-  </si>
-  <si>
-    <t>61001</t>
-  </si>
-  <si>
-    <t>32306</t>
-  </si>
-  <si>
-    <t>CVETNI PRAH V VREČKI 150 g</t>
-  </si>
-  <si>
-    <t>Naravni čebelji pridelek</t>
-  </si>
-  <si>
-    <t>Cvetni prah 100 %</t>
-  </si>
-  <si>
-    <t>Granule različne barve od rumene, rdeče, rjave do sive, različnih oblik in velikosti</t>
-  </si>
-  <si>
-    <t>Grenko sladkega okusa</t>
-  </si>
-  <si>
-    <t>Izdelek je v skladu z nacionalno in evropsko zakonodajo Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
-  </si>
-  <si>
-    <t>&lt; 10.000/g</t>
-  </si>
-  <si>
-    <t>≤ 9,0 %</t>
+    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
+  </si>
+  <si>
+    <t>Kartonska škatla</t>
+  </si>
+  <si>
+    <t>110x40x190</t>
+  </si>
+  <si>
+    <t>110x400x190</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>15 mesecev</t>
+  </si>
+  <si>
+    <t>V suhem prostoru.</t>
   </si>
   <si>
     <t>32333</t>
@@ -299,58 +487,31 @@
     <t>['364', 'kcal']</t>
   </si>
   <si>
-    <t>['0', 'g']</t>
-  </si>
-  <si>
     <t>['17', 'g']</t>
   </si>
   <si>
     <t>['0,6', 'g']</t>
   </si>
   <si>
+    <t>['72', 'g']</t>
+  </si>
+  <si>
     <t>['2,7', 'g']</t>
   </si>
   <si>
-    <t>['72', 'g']</t>
-  </si>
-  <si>
-    <t>30140</t>
-  </si>
-  <si>
-    <t>MED AKACIJEV S TARTUFI 250 G</t>
-  </si>
-  <si>
-    <t>Akacijev med s tartufi</t>
-  </si>
-  <si>
-    <t>Akacijev med 99 %, črni tartufi (Tuber aestivum) 1 %</t>
-  </si>
-  <si>
-    <t>Gosta, viskozna tekočina rumene barve, z rjavimi, črnimi koščki tartufov na vrhu kozarca</t>
-  </si>
-  <si>
-    <t>Prevladujoča, značilna za tartufe</t>
-  </si>
-  <si>
-    <t>Izdelek je v skladu z veljavno nacionalno in evropsko zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
-  </si>
-  <si>
-    <t>['1429', 'kJ']</t>
-  </si>
-  <si>
-    <t>['336', 'kcal']</t>
-  </si>
-  <si>
-    <t>['0,4', 'g']</t>
-  </si>
-  <si>
-    <t>['83', 'g']</t>
-  </si>
-  <si>
-    <t>['0,2', 'g']</t>
-  </si>
-  <si>
-    <t>['0,018', 'g']</t>
+    <t>pločevinka</t>
+  </si>
+  <si>
+    <t>80x80x115</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>245x165x115</t>
+  </si>
+  <si>
+    <t>36 mesecev</t>
   </si>
 </sst>
 </file>
@@ -699,7 +860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,7 +868,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,60 +962,94 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s"/>
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
+      </c>
       <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>42</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="O2" t="s"/>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T2" t="s">
-        <v>44</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="T2" t="s"/>
       <c r="U2" t="s"/>
       <c r="V2" t="s"/>
       <c r="W2" t="s"/>
@@ -866,58 +1061,92 @@
       <c r="AC2" t="s"/>
       <c r="AD2" t="s"/>
       <c r="AE2" t="s"/>
+      <c r="AF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP2" t="s"/>
+      <c r="AQ2" t="s"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" t="s">
         <v>53</v>
       </c>
+      <c r="M3" t="s"/>
       <c r="N3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" t="s"/>
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>70</v>
+      </c>
       <c r="P3" t="s"/>
       <c r="Q3" t="s"/>
       <c r="R3" t="s"/>
       <c r="S3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" t="s"/>
+        <v>71</v>
+      </c>
+      <c r="T3" t="s">
+        <v>72</v>
+      </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s"/>
       <c r="W3" t="s"/>
@@ -929,29 +1158,51 @@
       <c r="AC3" t="s"/>
       <c r="AD3" t="s"/>
       <c r="AE3" t="s"/>
+      <c r="AF3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP3" t="s"/>
+      <c r="AQ3" t="s"/>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B4" t="s"/>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D4" t="s"/>
+      <c r="E4" t="s"/>
+      <c r="F4" t="s"/>
+      <c r="G4" t="s"/>
       <c r="H4" t="s"/>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
@@ -967,60 +1218,80 @@
       <c r="T4" t="s"/>
       <c r="U4" t="s"/>
       <c r="V4" t="s"/>
-      <c r="W4" t="s">
-        <v>61</v>
-      </c>
-      <c r="X4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="W4" t="s"/>
+      <c r="X4" t="s"/>
+      <c r="Y4" t="s"/>
+      <c r="Z4" t="s"/>
+      <c r="AA4" t="s"/>
+      <c r="AB4" t="s"/>
+      <c r="AC4" t="s"/>
+      <c r="AD4" t="s"/>
+      <c r="AE4" t="s"/>
+      <c r="AF4" t="s"/>
+      <c r="AG4" t="s"/>
+      <c r="AH4" t="s"/>
+      <c r="AI4" t="s"/>
+      <c r="AJ4" t="s"/>
+      <c r="AK4" t="s"/>
+      <c r="AL4" t="s"/>
+      <c r="AM4" t="s"/>
+      <c r="AN4" t="s"/>
+      <c r="AO4" t="s"/>
+      <c r="AP4" t="s"/>
+      <c r="AQ4" t="s"/>
+    </row>
+    <row r="5" spans="1:43">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" t="s">
         <v>68</v>
       </c>
-      <c r="AE4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s"/>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="s"/>
-      <c r="F5" t="s"/>
-      <c r="G5" t="s"/>
-      <c r="H5" t="s"/>
-      <c r="I5" t="s"/>
-      <c r="J5" t="s"/>
-      <c r="K5" t="s"/>
-      <c r="L5" t="s"/>
+      <c r="J5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
       <c r="M5" t="s"/>
       <c r="N5" t="s"/>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s"/>
+      <c r="O5" t="s">
+        <v>70</v>
+      </c>
+      <c r="P5" t="s">
+        <v>68</v>
+      </c>
       <c r="Q5" t="s"/>
       <c r="R5" t="s"/>
       <c r="S5" t="s"/>
       <c r="T5" t="s"/>
-      <c r="U5" t="s"/>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
       <c r="V5" t="s"/>
       <c r="W5" t="s"/>
       <c r="X5" t="s"/>
@@ -1031,227 +1302,361 @@
       <c r="AC5" t="s"/>
       <c r="AD5" t="s"/>
       <c r="AE5" t="s"/>
+      <c r="AF5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP5" t="s"/>
+      <c r="AQ5" t="s"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>78</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="K6" t="s"/>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="M6" t="s"/>
-      <c r="N6" t="s"/>
+      <c r="N6" t="s">
+        <v>68</v>
+      </c>
       <c r="O6" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" t="s"/>
+        <v>70</v>
+      </c>
+      <c r="P6" t="s"/>
+      <c r="Q6" t="s">
+        <v>69</v>
+      </c>
       <c r="R6" t="s"/>
       <c r="S6" t="s"/>
       <c r="T6" t="s"/>
-      <c r="U6" t="s">
-        <v>79</v>
-      </c>
+      <c r="U6" t="s"/>
       <c r="V6" t="s"/>
-      <c r="W6" t="s"/>
-      <c r="X6" t="s"/>
-      <c r="Y6" t="s"/>
-      <c r="Z6" t="s"/>
-      <c r="AA6" t="s"/>
-      <c r="AB6" t="s"/>
-      <c r="AC6" t="s"/>
-      <c r="AD6" t="s"/>
+      <c r="W6" t="s">
+        <v>105</v>
+      </c>
+      <c r="X6" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>111</v>
+      </c>
       <c r="AE6" t="s"/>
+      <c r="AF6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ6" t="s"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="H7" t="s"/>
       <c r="I7" t="s"/>
       <c r="J7" t="s"/>
       <c r="K7" t="s"/>
-      <c r="L7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N7" t="s">
-        <v>87</v>
-      </c>
-      <c r="O7" t="s">
-        <v>88</v>
-      </c>
+      <c r="L7" t="s"/>
+      <c r="M7" t="s"/>
+      <c r="N7" t="s"/>
+      <c r="O7" t="s"/>
       <c r="P7" t="s"/>
-      <c r="Q7" t="s">
-        <v>89</v>
-      </c>
+      <c r="Q7" t="s"/>
       <c r="R7" t="s"/>
       <c r="S7" t="s"/>
       <c r="T7" t="s"/>
-      <c r="U7" t="s">
+      <c r="U7" t="s"/>
+      <c r="V7" t="s"/>
+      <c r="W7" t="s">
+        <v>126</v>
+      </c>
+      <c r="X7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF7" t="s">
         <v>90</v>
       </c>
-      <c r="V7" t="s">
-        <v>91</v>
-      </c>
-      <c r="W7" t="s">
-        <v>92</v>
-      </c>
-      <c r="X7" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>96</v>
+      <c r="AG7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP7" t="s"/>
+      <c r="AQ7" t="s">
+        <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="H8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" t="s">
-        <v>39</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I8" t="s"/>
+      <c r="J8" t="s"/>
       <c r="K8" t="s"/>
       <c r="L8" t="s">
-        <v>41</v>
-      </c>
-      <c r="M8" t="s"/>
+        <v>53</v>
+      </c>
+      <c r="M8" t="s">
+        <v>149</v>
+      </c>
       <c r="N8" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="O8" t="s">
-        <v>42</v>
+        <v>151</v>
       </c>
       <c r="P8" t="s"/>
       <c r="Q8" t="s"/>
       <c r="R8" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="S8" t="s"/>
       <c r="T8" t="s"/>
-      <c r="U8" t="s"/>
-      <c r="V8" t="s"/>
+      <c r="U8" t="s">
+        <v>153</v>
+      </c>
+      <c r="V8" t="s">
+        <v>154</v>
+      </c>
       <c r="W8" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="X8" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="Y8" t="s">
         <v>108</v>
       </c>
       <c r="Z8" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="AA8" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="AB8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC8" t="s"/>
+        <v>158</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>159</v>
+      </c>
       <c r="AD8" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="AE8" t="s">
-        <v>111</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AP8" t="s"/>
+      <c r="AQ8" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
now just need to fine tune
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="182">
   <si>
     <t>Šifra</t>
   </si>
@@ -109,6 +109,27 @@
     <t>Prehranske vlaknine</t>
   </si>
   <si>
+    <t>Izvleček smrekovih vršičkov</t>
+  </si>
+  <si>
+    <t>Kofein iz gvarane</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Vitamin A</t>
+  </si>
+  <si>
+    <t>niacin</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance®</t>
+  </si>
+  <si>
+    <t>Magnezij</t>
+  </si>
+  <si>
     <t>neto</t>
   </si>
   <si>
@@ -184,6 +205,12 @@
     <t>1,1660 g/ml (1,1427 – 1,1893) g/ml</t>
   </si>
   <si>
+    <t>['100', 'mg']</t>
+  </si>
+  <si>
+    <t>['2,4', 'mg']</t>
+  </si>
+  <si>
     <t>45 ml (5 x 9 ml)</t>
   </si>
   <si>
@@ -235,6 +262,18 @@
     <t>75,0 % (74,0 – 76,0) %</t>
   </si>
   <si>
+    <t>['180', 'mg']</t>
+  </si>
+  <si>
+    <t>['820', 'mg']</t>
+  </si>
+  <si>
+    <t>['32', 'g']</t>
+  </si>
+  <si>
+    <t>['240', 'μg']</t>
+  </si>
+  <si>
     <t>200 ml</t>
   </si>
   <si>
@@ -481,6 +520,9 @@
     <t>min. 0,8 %</t>
   </si>
   <si>
+    <t>['800', 'mg']</t>
+  </si>
+  <si>
     <t>['1523', 'kJ']</t>
   </si>
   <si>
@@ -497,6 +539,12 @@
   </si>
   <si>
     <t>['2,7', 'g']</t>
+  </si>
+  <si>
+    <t>['80', 'g']</t>
+  </si>
+  <si>
+    <t>['1875', 'mg']</t>
   </si>
   <si>
     <t>pločevinka</t>
@@ -860,7 +908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ8"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,7 +916,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,118 +984,148 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:53">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="O2" t="s"/>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s"/>
       <c r="U2" t="s"/>
@@ -1061,95 +1139,111 @@
       <c r="AC2" t="s"/>
       <c r="AD2" t="s"/>
       <c r="AE2" t="s"/>
-      <c r="AF2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AF2" t="s"/>
+      <c r="AG2" t="s"/>
+      <c r="AH2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" t="s"/>
+      <c r="AJ2" t="s"/>
+      <c r="AK2" t="s"/>
+      <c r="AL2" t="s"/>
+      <c r="AM2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN2" t="s"/>
+      <c r="AO2" t="s"/>
+      <c r="AP2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ2" t="s"/>
+      <c r="BA2" t="s"/>
+    </row>
+    <row r="3" spans="1:53">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
         <v>57</v>
       </c>
-      <c r="AH2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" t="s">
         <v>60</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" t="s"/>
-      <c r="AQ2" t="s"/>
-    </row>
-    <row r="3" spans="1:43">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
       </c>
       <c r="M3" t="s"/>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s"/>
       <c r="Q3" t="s"/>
       <c r="R3" t="s"/>
       <c r="S3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="T3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s"/>
-      <c r="W3" t="s"/>
+      <c r="W3" t="s">
+        <v>82</v>
+      </c>
       <c r="X3" t="s"/>
       <c r="Y3" t="s"/>
       <c r="Z3" t="s"/>
@@ -1158,46 +1252,64 @@
       <c r="AC3" t="s"/>
       <c r="AD3" t="s"/>
       <c r="AE3" t="s"/>
-      <c r="AF3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AF3" t="s"/>
       <c r="AG3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>75</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="AH3" t="s"/>
       <c r="AI3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AJ3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>75</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="AK3" t="s"/>
       <c r="AL3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP3" t="s"/>
-      <c r="AQ3" t="s"/>
+        <v>82</v>
+      </c>
+      <c r="AM3" t="s"/>
+      <c r="AN3" t="s"/>
+      <c r="AO3" t="s"/>
+      <c r="AP3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" t="s"/>
+      <c r="BA3" t="s"/>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:53">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s"/>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s"/>
       <c r="E4" t="s"/>
@@ -1239,58 +1351,68 @@
       <c r="AO4" t="s"/>
       <c r="AP4" t="s"/>
       <c r="AQ4" t="s"/>
+      <c r="AR4" t="s"/>
+      <c r="AS4" t="s"/>
+      <c r="AT4" t="s"/>
+      <c r="AU4" t="s"/>
+      <c r="AV4" t="s"/>
+      <c r="AW4" t="s"/>
+      <c r="AX4" t="s"/>
+      <c r="AY4" t="s"/>
+      <c r="AZ4" t="s"/>
+      <c r="BA4" t="s"/>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:53">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s"/>
       <c r="N5" t="s"/>
       <c r="O5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P5" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="Q5" t="s"/>
       <c r="R5" t="s"/>
       <c r="S5" t="s"/>
       <c r="T5" t="s"/>
       <c r="U5" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="V5" t="s"/>
       <c r="W5" t="s"/>
@@ -1302,171 +1424,191 @@
       <c r="AC5" t="s"/>
       <c r="AD5" t="s"/>
       <c r="AE5" t="s"/>
-      <c r="AF5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AP5" t="s"/>
-      <c r="AQ5" t="s"/>
+      <c r="AF5" t="s"/>
+      <c r="AG5" t="s"/>
+      <c r="AH5" t="s"/>
+      <c r="AI5" t="s"/>
+      <c r="AJ5" t="s"/>
+      <c r="AK5" t="s"/>
+      <c r="AL5" t="s"/>
+      <c r="AM5" t="s"/>
+      <c r="AN5" t="s"/>
+      <c r="AO5" t="s"/>
+      <c r="AP5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AZ5" t="s"/>
+      <c r="BA5" t="s"/>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:53">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s"/>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="P6" t="s"/>
       <c r="Q6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="R6" t="s"/>
       <c r="S6" t="s"/>
       <c r="T6" t="s"/>
       <c r="U6" t="s"/>
       <c r="V6" t="s"/>
-      <c r="W6" t="s">
-        <v>105</v>
-      </c>
+      <c r="W6" t="s"/>
       <c r="X6" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="Y6" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="Z6" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="AA6" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="AB6" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="AC6" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="AD6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE6" t="s"/>
-      <c r="AF6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>118</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>61</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF6" t="s"/>
+      <c r="AG6" t="s"/>
+      <c r="AH6" t="s"/>
+      <c r="AI6" t="s"/>
+      <c r="AJ6" t="s"/>
+      <c r="AK6" t="s"/>
+      <c r="AL6" t="s"/>
+      <c r="AM6" t="s"/>
+      <c r="AN6" t="s"/>
+      <c r="AO6" t="s"/>
       <c r="AP6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ6" t="s"/>
+        <v>125</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>132</v>
+      </c>
+      <c r="BA6" t="s"/>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:53">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="H7" t="s"/>
       <c r="I7" t="s"/>
@@ -1483,180 +1625,210 @@
       <c r="T7" t="s"/>
       <c r="U7" t="s"/>
       <c r="V7" t="s"/>
-      <c r="W7" t="s">
-        <v>126</v>
-      </c>
+      <c r="W7" t="s"/>
       <c r="X7" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="Y7" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="Z7" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="AA7" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="AB7" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="AC7" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="AD7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="AE7" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="AF7" t="s">
-        <v>90</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>138</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AP7" t="s"/>
+        <v>147</v>
+      </c>
+      <c r="AG7" t="s"/>
+      <c r="AH7" t="s"/>
+      <c r="AI7" t="s"/>
+      <c r="AJ7" t="s"/>
+      <c r="AK7" t="s"/>
+      <c r="AL7" t="s"/>
+      <c r="AM7" t="s"/>
+      <c r="AN7" t="s"/>
+      <c r="AO7" t="s"/>
+      <c r="AP7" t="s">
+        <v>103</v>
+      </c>
       <c r="AQ7" t="s">
-        <v>142</v>
+        <v>148</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AZ7" t="s"/>
+      <c r="BA7" t="s">
+        <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:53">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="F8" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="G8" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s"/>
       <c r="J8" t="s"/>
       <c r="K8" t="s"/>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="M8" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="N8" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="O8" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="P8" t="s"/>
       <c r="Q8" t="s"/>
       <c r="R8" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="S8" t="s"/>
       <c r="T8" t="s"/>
       <c r="U8" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="V8" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="W8" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="X8" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="Y8" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="Z8" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="AA8" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="AB8" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="AC8" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="AD8" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="AE8" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="AF8" t="s">
-        <v>90</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>162</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>45</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="AG8" t="s"/>
+      <c r="AH8" t="s"/>
+      <c r="AI8" t="s"/>
+      <c r="AJ8" t="s"/>
       <c r="AK8" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="AL8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>164</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="AM8" t="s"/>
       <c r="AN8" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="AO8" t="s">
-        <v>165</v>
-      </c>
-      <c r="AP8" t="s"/>
-      <c r="AQ8" t="s"/>
+        <v>176</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>178</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>181</v>
+      </c>
+      <c r="AZ8" t="s"/>
+      <c r="BA8" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
added tools to filter wrong doc types and most recent document
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1034,7 +1034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BZ8"/>
+  <dimension ref="A1:BZ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2156,35 +2156,47 @@
     </row>
     <row r="8" spans="1:78">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
       <c r="G8" t="s">
-        <v>203</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
         <v>85</v>
       </c>
-      <c r="I8" t="s"/>
-      <c r="J8" t="s"/>
-      <c r="K8" t="s"/>
-      <c r="L8" t="s"/>
-      <c r="M8" t="s"/>
-      <c r="N8" t="s"/>
+      <c r="I8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" t="s">
+        <v>88</v>
+      </c>
+      <c r="N8" t="s">
+        <v>87</v>
+      </c>
       <c r="O8" t="s">
         <v>89</v>
       </c>
@@ -2192,157 +2204,299 @@
         <v>90</v>
       </c>
       <c r="Q8" t="s">
-        <v>204</v>
+        <v>91</v>
       </c>
       <c r="R8" t="s">
-        <v>205</v>
+        <v>92</v>
       </c>
       <c r="S8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T8" t="s">
-        <v>206</v>
-      </c>
-      <c r="U8" t="s">
-        <v>207</v>
-      </c>
-      <c r="V8" t="s">
-        <v>205</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="U8" t="s"/>
+      <c r="V8" t="s"/>
       <c r="W8" t="s"/>
       <c r="X8" t="s"/>
       <c r="Y8" t="s"/>
       <c r="Z8" t="s"/>
-      <c r="AA8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>205</v>
-      </c>
-      <c r="AC8" t="s"/>
+      <c r="AA8" t="s"/>
+      <c r="AB8" t="s"/>
+      <c r="AC8" t="s">
+        <v>93</v>
+      </c>
       <c r="AD8" t="s"/>
-      <c r="AE8" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>209</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>211</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>212</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>213</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>214</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>213</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX8" t="s">
-        <v>119</v>
-      </c>
+      <c r="AE8" t="s"/>
+      <c r="AF8" t="s"/>
+      <c r="AG8" t="s"/>
+      <c r="AH8" t="s"/>
+      <c r="AI8" t="s"/>
+      <c r="AJ8" t="s"/>
+      <c r="AK8" t="s"/>
+      <c r="AL8" t="s"/>
+      <c r="AM8" t="s"/>
+      <c r="AN8" t="s"/>
+      <c r="AO8" t="s"/>
+      <c r="AP8" t="s"/>
+      <c r="AQ8" t="s"/>
+      <c r="AR8" t="s"/>
+      <c r="AS8" t="s"/>
+      <c r="AT8" t="s"/>
+      <c r="AU8" t="s"/>
+      <c r="AV8" t="s"/>
+      <c r="AW8" t="s"/>
+      <c r="AX8" t="s"/>
       <c r="AY8" t="s"/>
       <c r="AZ8" t="s"/>
-      <c r="BA8" t="s"/>
-      <c r="BB8" t="s"/>
+      <c r="BA8" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>95</v>
+      </c>
       <c r="BC8" t="s"/>
       <c r="BD8" t="s"/>
       <c r="BE8" t="s"/>
       <c r="BF8" t="s"/>
-      <c r="BG8" t="s">
-        <v>216</v>
-      </c>
-      <c r="BH8" t="s">
+      <c r="BG8" t="s"/>
+      <c r="BH8" t="s"/>
+      <c r="BI8" t="s">
+        <v>96</v>
+      </c>
+      <c r="BJ8" t="s">
         <v>95</v>
       </c>
-      <c r="BI8" t="s"/>
-      <c r="BJ8" t="s"/>
-      <c r="BK8" t="s">
-        <v>217</v>
-      </c>
-      <c r="BL8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BM8" t="s">
-        <v>218</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>95</v>
-      </c>
+      <c r="BK8" t="s"/>
+      <c r="BL8" t="s"/>
+      <c r="BM8" t="s"/>
+      <c r="BN8" t="s"/>
       <c r="BO8" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="BP8" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="BQ8" t="s">
         <v>80</v>
       </c>
       <c r="BR8" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="BS8" t="s">
         <v>80</v>
       </c>
       <c r="BT8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>100</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BW8" t="s">
+        <v>101</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:78">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s"/>
+      <c r="J9" t="s"/>
+      <c r="K9" t="s"/>
+      <c r="L9" t="s"/>
+      <c r="M9" t="s"/>
+      <c r="N9" t="s"/>
+      <c r="O9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>204</v>
+      </c>
+      <c r="R9" t="s">
+        <v>205</v>
+      </c>
+      <c r="S9" t="s">
+        <v>89</v>
+      </c>
+      <c r="T9" t="s">
+        <v>206</v>
+      </c>
+      <c r="U9" t="s">
+        <v>207</v>
+      </c>
+      <c r="V9" t="s">
+        <v>205</v>
+      </c>
+      <c r="W9" t="s"/>
+      <c r="X9" t="s"/>
+      <c r="Y9" t="s"/>
+      <c r="Z9" t="s"/>
+      <c r="AA9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC9" t="s"/>
+      <c r="AD9" t="s"/>
+      <c r="AE9" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>212</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>213</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>213</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY9" t="s"/>
+      <c r="AZ9" t="s"/>
+      <c r="BA9" t="s"/>
+      <c r="BB9" t="s"/>
+      <c r="BC9" t="s"/>
+      <c r="BD9" t="s"/>
+      <c r="BE9" t="s"/>
+      <c r="BF9" t="s"/>
+      <c r="BG9" t="s">
+        <v>216</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BI9" t="s"/>
+      <c r="BJ9" t="s"/>
+      <c r="BK9" t="s">
+        <v>217</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>218</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>142</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>219</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>220</v>
+      </c>
+      <c r="BS9" t="s">
+        <v>80</v>
+      </c>
+      <c r="BT9" t="s">
         <v>125</v>
       </c>
-      <c r="BU8" t="s">
+      <c r="BU9" t="s">
         <v>221</v>
       </c>
-      <c r="BV8" t="s">
+      <c r="BV9" t="s">
         <v>222</v>
       </c>
-      <c r="BW8" t="s">
+      <c r="BW9" t="s">
         <v>173</v>
       </c>
-      <c r="BX8" t="s">
+      <c r="BX9" t="s">
         <v>149</v>
       </c>
-      <c r="BY8" t="s">
+      <c r="BY9" t="s">
         <v>223</v>
       </c>
-      <c r="BZ8" t="s">
+      <c r="BZ9" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started to process unstructured document (with just text)
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="224">
   <si>
     <t>Šifra</t>
   </si>
@@ -52,54 +53,54 @@
     <t>Escherichia coli enote</t>
   </si>
   <si>
+    <t>Plesni in kvasovke</t>
+  </si>
+  <si>
+    <t>Plesni in kvasovke enote</t>
+  </si>
+  <si>
+    <t>Salmonella</t>
+  </si>
+  <si>
+    <t>Salmonella enote</t>
+  </si>
+  <si>
+    <t>Skupno število</t>
+  </si>
+  <si>
+    <t>Skupno število enote</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus enote</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji enote</t>
+  </si>
+  <si>
     <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus</t>
   </si>
   <si>
     <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus enote</t>
   </si>
   <si>
+    <t>Enterobakterije</t>
+  </si>
+  <si>
+    <t>Enterobakterije enote</t>
+  </si>
+  <si>
     <t>Kvasovke in plesni</t>
   </si>
   <si>
     <t>Kvasovke in plesni enote</t>
   </si>
   <si>
-    <t>Plesni in kvasovke</t>
-  </si>
-  <si>
-    <t>Plesni in kvasovke enote</t>
-  </si>
-  <si>
-    <t>Salmonella</t>
-  </si>
-  <si>
-    <t>Salmonella enote</t>
-  </si>
-  <si>
-    <t>Skupno število</t>
-  </si>
-  <si>
-    <t>Skupno število enote</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus enote</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji enote</t>
-  </si>
-  <si>
-    <t>Enterobakterije</t>
-  </si>
-  <si>
-    <t>Enterobakterije enote</t>
-  </si>
-  <si>
     <t>Gostota</t>
   </si>
   <si>
@@ -148,6 +149,12 @@
     <t>S Enote</t>
   </si>
   <si>
+    <t>Prehranske vlaknine</t>
+  </si>
+  <si>
+    <t>PV Enote</t>
+  </si>
+  <si>
     <t>Beljakovine</t>
   </si>
   <si>
@@ -160,12 +167,6 @@
     <t>Sol Enote</t>
   </si>
   <si>
-    <t>Prehranske vlaknine</t>
-  </si>
-  <si>
-    <t>PV Enote</t>
-  </si>
-  <si>
     <t>Izvleček smrekovih vršičkov(akt)</t>
   </si>
   <si>
@@ -412,6 +413,87 @@
     <t>6</t>
   </si>
   <si>
+    <t>40408</t>
+  </si>
+  <si>
+    <t>BIO keksi pomaranča 150 g</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
+  </si>
+  <si>
+    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
+  </si>
+  <si>
+    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
+  </si>
+  <si>
+    <t>1861</t>
+  </si>
+  <si>
+    <t>kJ</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
+    <t>kcal</t>
+  </si>
+  <si>
+    <t>16,6</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>63,5</t>
+  </si>
+  <si>
+    <t>21,7</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>8,1</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>110x400x190</t>
+  </si>
+  <si>
+    <t>110x40x190</t>
+  </si>
+  <si>
+    <t>V suhem prostoru.</t>
+  </si>
+  <si>
+    <t>150 g</t>
+  </si>
+  <si>
+    <t>15 mesecev</t>
+  </si>
+  <si>
+    <t>Kartonska škatla</t>
+  </si>
+  <si>
+    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>61001</t>
+  </si>
+  <si>
     <t>32306</t>
   </si>
   <si>
@@ -448,9 +530,6 @@
     <t>V temnem in suhem prostoru pri temperaturi 15-25 °C.</t>
   </si>
   <si>
-    <t>150 g</t>
-  </si>
-  <si>
     <t>18 mesecev</t>
   </si>
   <si>
@@ -466,6 +545,90 @@
     <t>5</t>
   </si>
   <si>
+    <t>32333</t>
+  </si>
+  <si>
+    <t>KOLAGENBODY 150 G</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
+  </si>
+  <si>
+    <t>Bel prah/granule</t>
+  </si>
+  <si>
+    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
+  </si>
+  <si>
+    <t>&lt; 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cfu/g</t>
+  </si>
+  <si>
+    <t>/1 g</t>
+  </si>
+  <si>
+    <t>&lt; 10</t>
+  </si>
+  <si>
+    <t>max. 8 %</t>
+  </si>
+  <si>
+    <t>min. 0,8 %</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>364</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>1875</t>
+  </si>
+  <si>
+    <t>245x165x115</t>
+  </si>
+  <si>
+    <t>80x80x115</t>
+  </si>
+  <si>
+    <t>36 mesecev</t>
+  </si>
+  <si>
+    <t>pločevinka</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>30140</t>
   </si>
   <si>
@@ -490,21 +653,12 @@
     <t>1429</t>
   </si>
   <si>
-    <t>kJ</t>
-  </si>
-  <si>
     <t>336</t>
   </si>
   <si>
-    <t>kcal</t>
-  </si>
-  <si>
     <t>0,4</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
@@ -533,156 +687,6 @@
   </si>
   <si>
     <t>1392</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>40408</t>
-  </si>
-  <si>
-    <t>BIO keksi pomaranča 150 g</t>
-  </si>
-  <si>
-    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
-  </si>
-  <si>
-    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
-  </si>
-  <si>
-    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
-  </si>
-  <si>
-    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
-  </si>
-  <si>
-    <t>1861</t>
-  </si>
-  <si>
-    <t>445</t>
-  </si>
-  <si>
-    <t>16,6</t>
-  </si>
-  <si>
-    <t>3,6</t>
-  </si>
-  <si>
-    <t>63,5</t>
-  </si>
-  <si>
-    <t>21,7</t>
-  </si>
-  <si>
-    <t>8,1</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>7,7</t>
-  </si>
-  <si>
-    <t>110x400x190</t>
-  </si>
-  <si>
-    <t>110x40x190</t>
-  </si>
-  <si>
-    <t>V suhem prostoru.</t>
-  </si>
-  <si>
-    <t>15 mesecev</t>
-  </si>
-  <si>
-    <t>Kartonska škatla</t>
-  </si>
-  <si>
-    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
-  </si>
-  <si>
-    <t>1920</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>32333</t>
-  </si>
-  <si>
-    <t>KOLAGENBODY 150 G</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
-  </si>
-  <si>
-    <t>Bel prah/granule</t>
-  </si>
-  <si>
-    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
-  </si>
-  <si>
-    <t>&lt; 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cfu/g</t>
-  </si>
-  <si>
-    <t>/1 g</t>
-  </si>
-  <si>
-    <t>&lt; 10</t>
-  </si>
-  <si>
-    <t>max. 8 %</t>
-  </si>
-  <si>
-    <t>min. 0,8 %</t>
-  </si>
-  <si>
-    <t>1523</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>0,6</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>2,7</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>1875</t>
-  </si>
-  <si>
-    <t>245x165x115</t>
-  </si>
-  <si>
-    <t>80x80x115</t>
-  </si>
-  <si>
-    <t>36 mesecev</t>
-  </si>
-  <si>
-    <t>pločevinka</t>
-  </si>
-  <si>
-    <t>1008</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BZ7"/>
+  <dimension ref="A1:BZ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1312,34 +1316,34 @@
       <c r="L2" t="s">
         <v>87</v>
       </c>
-      <c r="M2" t="s"/>
-      <c r="N2" t="s"/>
-      <c r="O2" t="s"/>
-      <c r="P2" t="s"/>
+      <c r="M2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
       <c r="Q2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" t="s">
         <v>87</v>
       </c>
-      <c r="S2" t="s">
-        <v>89</v>
-      </c>
-      <c r="T2" t="s">
-        <v>90</v>
-      </c>
-      <c r="U2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V2" t="s">
-        <v>92</v>
-      </c>
-      <c r="W2" t="s">
-        <v>86</v>
-      </c>
-      <c r="X2" t="s">
-        <v>87</v>
-      </c>
+      <c r="U2" t="s"/>
+      <c r="V2" t="s"/>
+      <c r="W2" t="s"/>
+      <c r="X2" t="s"/>
       <c r="Y2" t="s"/>
       <c r="Z2" t="s"/>
       <c r="AA2" t="s"/>
@@ -1466,36 +1470,36 @@
       <c r="L3" t="s">
         <v>111</v>
       </c>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s">
+      <c r="M3" t="s">
         <v>112</v>
       </c>
-      <c r="R3" t="s">
+      <c r="N3" t="s">
         <v>113</v>
       </c>
+      <c r="O3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" t="s"/>
+      <c r="R3" t="s"/>
       <c r="S3" t="s">
         <v>89</v>
       </c>
       <c r="T3" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" t="s"/>
-      <c r="V3" t="s"/>
-      <c r="W3" t="s">
+        <v>111</v>
+      </c>
+      <c r="U3" t="s">
         <v>89</v>
       </c>
-      <c r="X3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="V3" t="s">
         <v>114</v>
       </c>
+      <c r="W3" t="s"/>
+      <c r="X3" t="s"/>
+      <c r="Y3" t="s"/>
+      <c r="Z3" t="s"/>
       <c r="AA3" t="s"/>
       <c r="AB3" t="s"/>
       <c r="AC3" t="s">
@@ -1615,77 +1619,85 @@
       <c r="G4" t="s">
         <v>137</v>
       </c>
-      <c r="H4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" t="s">
-        <v>89</v>
-      </c>
-      <c r="N4" t="s">
-        <v>111</v>
-      </c>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s"/>
+      <c r="J4" t="s"/>
+      <c r="K4" t="s"/>
+      <c r="L4" t="s"/>
+      <c r="M4" t="s"/>
+      <c r="N4" t="s"/>
       <c r="O4" t="s"/>
       <c r="P4" t="s"/>
-      <c r="Q4" t="s">
-        <v>139</v>
-      </c>
-      <c r="R4" t="s">
-        <v>113</v>
-      </c>
-      <c r="S4" t="s">
-        <v>89</v>
-      </c>
-      <c r="T4" t="s">
-        <v>90</v>
-      </c>
+      <c r="Q4" t="s"/>
+      <c r="R4" t="s"/>
+      <c r="S4" t="s"/>
+      <c r="T4" t="s"/>
       <c r="U4" t="s"/>
       <c r="V4" t="s"/>
       <c r="W4" t="s"/>
       <c r="X4" t="s"/>
-      <c r="Y4" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>114</v>
-      </c>
+      <c r="Y4" t="s"/>
+      <c r="Z4" t="s"/>
       <c r="AA4" t="s"/>
       <c r="AB4" t="s"/>
       <c r="AC4" t="s"/>
       <c r="AD4" t="s"/>
-      <c r="AE4" t="s">
+      <c r="AE4" t="s"/>
+      <c r="AF4" t="s"/>
+      <c r="AG4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI4" t="s">
         <v>140</v>
       </c>
-      <c r="AF4" t="s"/>
-      <c r="AG4" t="s"/>
-      <c r="AH4" t="s"/>
-      <c r="AI4" t="s"/>
-      <c r="AJ4" t="s"/>
-      <c r="AK4" t="s"/>
-      <c r="AL4" t="s"/>
-      <c r="AM4" t="s"/>
-      <c r="AN4" t="s"/>
-      <c r="AO4" t="s"/>
-      <c r="AP4" t="s"/>
-      <c r="AQ4" t="s"/>
-      <c r="AR4" t="s"/>
-      <c r="AS4" t="s"/>
-      <c r="AT4" t="s"/>
-      <c r="AU4" t="s"/>
-      <c r="AV4" t="s"/>
-      <c r="AW4" t="s"/>
-      <c r="AX4" t="s"/>
+      <c r="AJ4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>119</v>
+      </c>
       <c r="AY4" t="s"/>
       <c r="AZ4" t="s"/>
       <c r="BA4" t="s"/>
@@ -1703,163 +1715,93 @@
       <c r="BM4" t="s"/>
       <c r="BN4" t="s"/>
       <c r="BO4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="BP4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="BQ4" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="BR4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>126</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="BS4" t="s"/>
       <c r="BT4" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="BU4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="BV4" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="BW4" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="BX4" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="BY4" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="BZ4" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:78">
       <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" t="s">
-        <v>151</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="B5" t="s"/>
       <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K5" t="s">
-        <v>89</v>
-      </c>
-      <c r="L5" t="s">
-        <v>111</v>
-      </c>
+      <c r="D5" t="s"/>
+      <c r="E5" t="s"/>
+      <c r="F5" t="s"/>
+      <c r="G5" t="s"/>
+      <c r="H5" t="s"/>
+      <c r="I5" t="s"/>
+      <c r="J5" t="s"/>
+      <c r="K5" t="s"/>
+      <c r="L5" t="s"/>
       <c r="M5" t="s"/>
       <c r="N5" t="s"/>
-      <c r="O5" t="s">
-        <v>112</v>
-      </c>
-      <c r="P5" t="s">
-        <v>113</v>
-      </c>
+      <c r="O5" t="s"/>
+      <c r="P5" t="s"/>
       <c r="Q5" t="s"/>
       <c r="R5" t="s"/>
-      <c r="S5" t="s">
-        <v>89</v>
-      </c>
-      <c r="T5" t="s">
-        <v>90</v>
-      </c>
+      <c r="S5" t="s"/>
+      <c r="T5" t="s"/>
       <c r="U5" t="s"/>
       <c r="V5" t="s"/>
-      <c r="W5" t="s">
-        <v>89</v>
-      </c>
-      <c r="X5" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>114</v>
-      </c>
+      <c r="W5" t="s"/>
+      <c r="X5" t="s"/>
+      <c r="Y5" t="s"/>
+      <c r="Z5" t="s"/>
       <c r="AA5" t="s"/>
       <c r="AB5" t="s"/>
       <c r="AC5" t="s"/>
       <c r="AD5" t="s"/>
       <c r="AE5" t="s"/>
       <c r="AF5" t="s"/>
-      <c r="AG5" t="s">
-        <v>157</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>160</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>161</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>162</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>163</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>163</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>164</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>165</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>119</v>
-      </c>
+      <c r="AG5" t="s"/>
+      <c r="AH5" t="s"/>
+      <c r="AI5" t="s"/>
+      <c r="AJ5" t="s"/>
+      <c r="AK5" t="s"/>
+      <c r="AL5" t="s"/>
+      <c r="AM5" t="s"/>
+      <c r="AN5" t="s"/>
+      <c r="AO5" t="s"/>
+      <c r="AP5" t="s"/>
+      <c r="AQ5" t="s"/>
+      <c r="AR5" t="s"/>
+      <c r="AS5" t="s"/>
+      <c r="AT5" t="s"/>
+      <c r="AU5" t="s"/>
+      <c r="AV5" t="s"/>
       <c r="AW5" t="s"/>
       <c r="AX5" t="s"/>
       <c r="AY5" t="s"/>
@@ -1878,144 +1820,112 @@
       <c r="BL5" t="s"/>
       <c r="BM5" t="s"/>
       <c r="BN5" t="s"/>
-      <c r="BO5" t="s">
-        <v>166</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>167</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>166</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>168</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>126</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>169</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>101</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>170</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>171</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>170</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>172</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>173</v>
-      </c>
+      <c r="BO5" t="s"/>
+      <c r="BP5" t="s"/>
+      <c r="BQ5" t="s"/>
+      <c r="BR5" t="s"/>
+      <c r="BS5" t="s"/>
+      <c r="BT5" t="s"/>
+      <c r="BU5" t="s"/>
+      <c r="BV5" t="s"/>
+      <c r="BW5" t="s"/>
+      <c r="BX5" t="s"/>
+      <c r="BY5" t="s"/>
+      <c r="BZ5" t="s"/>
     </row>
     <row r="6" spans="1:78">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="G6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" t="s"/>
-      <c r="I6" t="s"/>
-      <c r="J6" t="s"/>
-      <c r="K6" t="s"/>
-      <c r="L6" t="s"/>
-      <c r="M6" t="s"/>
-      <c r="N6" t="s"/>
-      <c r="O6" t="s"/>
-      <c r="P6" t="s"/>
+        <v>164</v>
+      </c>
+      <c r="H6" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" t="s">
+        <v>166</v>
+      </c>
+      <c r="N6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O6" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" t="s">
+        <v>90</v>
+      </c>
       <c r="Q6" t="s"/>
       <c r="R6" t="s"/>
       <c r="S6" t="s"/>
       <c r="T6" t="s"/>
-      <c r="U6" t="s"/>
-      <c r="V6" t="s"/>
-      <c r="W6" t="s"/>
-      <c r="X6" t="s"/>
+      <c r="U6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" t="s">
+        <v>114</v>
+      </c>
+      <c r="W6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X6" t="s">
+        <v>111</v>
+      </c>
       <c r="Y6" t="s"/>
       <c r="Z6" t="s"/>
       <c r="AA6" t="s"/>
       <c r="AB6" t="s"/>
       <c r="AC6" t="s"/>
       <c r="AD6" t="s"/>
-      <c r="AE6" t="s"/>
+      <c r="AE6" t="s">
+        <v>167</v>
+      </c>
       <c r="AF6" t="s"/>
-      <c r="AG6" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>158</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>181</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>160</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>183</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>184</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>186</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>187</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>188</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>119</v>
-      </c>
+      <c r="AG6" t="s"/>
+      <c r="AH6" t="s"/>
+      <c r="AI6" t="s"/>
+      <c r="AJ6" t="s"/>
+      <c r="AK6" t="s"/>
+      <c r="AL6" t="s"/>
+      <c r="AM6" t="s"/>
+      <c r="AN6" t="s"/>
+      <c r="AO6" t="s"/>
+      <c r="AP6" t="s"/>
+      <c r="AQ6" t="s"/>
+      <c r="AR6" t="s"/>
+      <c r="AS6" t="s"/>
+      <c r="AT6" t="s"/>
+      <c r="AU6" t="s"/>
+      <c r="AV6" t="s"/>
+      <c r="AW6" t="s"/>
+      <c r="AX6" t="s"/>
       <c r="AY6" t="s"/>
       <c r="AZ6" t="s"/>
       <c r="BA6" t="s"/>
@@ -2033,61 +1943,63 @@
       <c r="BM6" t="s"/>
       <c r="BN6" t="s"/>
       <c r="BO6" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="BP6" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="BQ6" t="s">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="BR6" t="s">
-        <v>191</v>
-      </c>
-      <c r="BS6" t="s"/>
+        <v>170</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>126</v>
+      </c>
       <c r="BT6" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="BU6" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="BV6" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="BW6" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="BX6" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="BY6" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="BZ6" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:78">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F7" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="G7" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="H7" t="s">
         <v>85</v>
@@ -2098,98 +2010,98 @@
       <c r="L7" t="s"/>
       <c r="M7" t="s"/>
       <c r="N7" t="s"/>
-      <c r="O7" t="s"/>
-      <c r="P7" t="s"/>
-      <c r="Q7" t="s"/>
-      <c r="R7" t="s"/>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>182</v>
+      </c>
+      <c r="R7" t="s">
+        <v>183</v>
+      </c>
       <c r="S7" t="s">
         <v>89</v>
       </c>
       <c r="T7" t="s">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="U7" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="V7" t="s">
-        <v>204</v>
-      </c>
-      <c r="W7" t="s">
-        <v>89</v>
-      </c>
-      <c r="X7" t="s">
-        <v>205</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="W7" t="s"/>
+      <c r="X7" t="s"/>
       <c r="Y7" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="Z7" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>204</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="AA7" t="s"/>
+      <c r="AB7" t="s"/>
       <c r="AC7" t="s"/>
       <c r="AD7" t="s"/>
       <c r="AE7" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="AF7" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="AG7" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="AH7" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="AI7" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="AJ7" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="AK7" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="AL7" t="s">
         <v>119</v>
       </c>
       <c r="AM7" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="AN7" t="s">
         <v>119</v>
       </c>
       <c r="AO7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="AP7" t="s">
         <v>119</v>
       </c>
       <c r="AQ7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="AR7" t="s">
         <v>119</v>
       </c>
       <c r="AS7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="AT7" t="s">
         <v>119</v>
       </c>
       <c r="AU7" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="AV7" t="s">
         <v>119</v>
       </c>
       <c r="AW7" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="AX7" t="s">
         <v>119</v>
@@ -2203,7 +2115,7 @@
       <c r="BE7" t="s"/>
       <c r="BF7" t="s"/>
       <c r="BG7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="BH7" t="s">
         <v>95</v>
@@ -2211,52 +2123,228 @@
       <c r="BI7" t="s"/>
       <c r="BJ7" t="s"/>
       <c r="BK7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="BL7" t="s">
         <v>119</v>
       </c>
       <c r="BM7" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="BN7" t="s">
         <v>95</v>
       </c>
       <c r="BO7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="BP7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="BQ7" t="s">
         <v>80</v>
       </c>
       <c r="BR7" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="BS7" t="s">
         <v>126</v>
       </c>
       <c r="BT7" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="BU7" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="BV7" t="s">
         <v>128</v>
       </c>
       <c r="BW7" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="BX7" t="s">
         <v>80</v>
       </c>
       <c r="BY7" t="s">
+        <v>202</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:78">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M8" t="s"/>
+      <c r="N8" t="s"/>
+      <c r="O8" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" t="s"/>
+      <c r="R8" t="s"/>
+      <c r="S8" t="s">
+        <v>89</v>
+      </c>
+      <c r="T8" t="s">
+        <v>111</v>
+      </c>
+      <c r="U8" t="s">
+        <v>89</v>
+      </c>
+      <c r="V8" t="s">
+        <v>114</v>
+      </c>
+      <c r="W8" t="s"/>
+      <c r="X8" t="s"/>
+      <c r="Y8" t="s"/>
+      <c r="Z8" t="s"/>
+      <c r="AA8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC8" t="s"/>
+      <c r="AD8" t="s"/>
+      <c r="AE8" t="s"/>
+      <c r="AF8" t="s"/>
+      <c r="AG8" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>214</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS8" t="s"/>
+      <c r="AT8" t="s"/>
+      <c r="AU8" t="s">
+        <v>215</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>216</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY8" t="s"/>
+      <c r="AZ8" t="s"/>
+      <c r="BA8" t="s"/>
+      <c r="BB8" t="s"/>
+      <c r="BC8" t="s"/>
+      <c r="BD8" t="s"/>
+      <c r="BE8" t="s"/>
+      <c r="BF8" t="s"/>
+      <c r="BG8" t="s"/>
+      <c r="BH8" t="s"/>
+      <c r="BI8" t="s"/>
+      <c r="BJ8" t="s"/>
+      <c r="BK8" t="s"/>
+      <c r="BL8" t="s"/>
+      <c r="BM8" t="s"/>
+      <c r="BN8" t="s"/>
+      <c r="BO8" t="s">
+        <v>217</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>218</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>217</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>219</v>
+      </c>
+      <c r="BS8" t="s">
+        <v>126</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>101</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>221</v>
+      </c>
+      <c r="BW8" t="s">
         <v>222</v>
       </c>
-      <c r="BZ7" t="s">
-        <v>173</v>
+      <c r="BX8" t="s">
+        <v>221</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>223</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
helu do u know da way
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="223">
   <si>
     <t>Šifra</t>
   </si>
@@ -88,18 +89,18 @@
     <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus enote</t>
   </si>
   <si>
+    <t>Enterobakterije</t>
+  </si>
+  <si>
+    <t>Enterobakterije enote</t>
+  </si>
+  <si>
     <t>Kvasovke in plesni</t>
   </si>
   <si>
     <t>Kvasovke in plesni enote</t>
   </si>
   <si>
-    <t>Enterobakterije</t>
-  </si>
-  <si>
-    <t>Enterobakterije enote</t>
-  </si>
-  <si>
     <t>Gostota</t>
   </si>
   <si>
@@ -148,6 +149,12 @@
     <t>S Enote</t>
   </si>
   <si>
+    <t>Prehranske vlaknine</t>
+  </si>
+  <si>
+    <t>PV Enote</t>
+  </si>
+  <si>
     <t>Beljakovine</t>
   </si>
   <si>
@@ -160,12 +167,6 @@
     <t>Sol Enote</t>
   </si>
   <si>
-    <t>Prehranske vlaknine</t>
-  </si>
-  <si>
-    <t>PV Enote</t>
-  </si>
-  <si>
     <t>Izvleček smrekovih vršičkov(akt)</t>
   </si>
   <si>
@@ -214,42 +215,42 @@
     <t>Magnezij(akt)Enote</t>
   </si>
   <si>
+    <t>dimenzija KP</t>
+  </si>
+  <si>
+    <t>dimenzija MPE</t>
+  </si>
+  <si>
+    <t>dimenzija TP</t>
+  </si>
+  <si>
+    <t>način skladiščenja</t>
+  </si>
+  <si>
+    <t>način transporta</t>
+  </si>
+  <si>
     <t>neto</t>
   </si>
   <si>
+    <t>rok uporabe</t>
+  </si>
+  <si>
+    <t>tip KP</t>
+  </si>
+  <si>
     <t>tip MPE</t>
   </si>
   <si>
     <t>tip TP</t>
   </si>
   <si>
-    <t>dimenzija MPE</t>
-  </si>
-  <si>
-    <t>dimenzija TP</t>
-  </si>
-  <si>
-    <t>tip KP</t>
-  </si>
-  <si>
     <t>število MPE</t>
   </si>
   <si>
-    <t>dimenzija KP</t>
-  </si>
-  <si>
     <t>število plasti na paleti</t>
   </si>
   <si>
-    <t>način skladiščenja</t>
-  </si>
-  <si>
-    <t>rok uporabe</t>
-  </si>
-  <si>
-    <t>način transporta</t>
-  </si>
-  <si>
     <t>32226</t>
   </si>
   <si>
@@ -307,30 +308,30 @@
     <t>2,4</t>
   </si>
   <si>
+    <t>127x115x24</t>
+  </si>
+  <si>
+    <t>V temnem in suhem prostoru pri temperaturi do 25 °C.</t>
+  </si>
+  <si>
+    <t>Zaščiteno pred vlago in mehanskimi poškodbami. Tovor je potrebno zaščititi pred drsenjem, udarci in prevračanjem</t>
+  </si>
+  <si>
     <t>45 ml (5 x 9 ml)</t>
   </si>
   <si>
+    <t>24 mesecev</t>
+  </si>
+  <si>
     <t>5 steklenih fiol s PP pokrovčki v plastičnem vložku in kartonski zloženki</t>
   </si>
   <si>
-    <t>127x115x24</t>
-  </si>
-  <si>
     <t>1800</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>V temnem in suhem prostoru pri temperaturi do 25 °C.</t>
-  </si>
-  <si>
-    <t>24 mesecev</t>
-  </si>
-  <si>
-    <t>Zaščiteno pred vlago in mehanskimi poškodbami. Tovor je potrebno zaščititi pred drsenjem, udarci in prevračanjem</t>
-  </si>
-  <si>
     <t>32348</t>
   </si>
   <si>
@@ -385,34 +386,109 @@
     <t>180</t>
   </si>
   <si>
+    <t>57x57x131</t>
+  </si>
+  <si>
+    <t>195x130x150</t>
+  </si>
+  <si>
+    <t>V temnem in suhem prostoru pri temperaturi 18-25 °C obrnjen s pokrovčkom navzgor.</t>
+  </si>
+  <si>
+    <t>Zaščiteno pred vlago in mehanskimi poškodbami. Tovor je potrebno zaščititi pred drsenjem, udarci in prevračanjem.</t>
+  </si>
+  <si>
     <t>200 ml</t>
   </si>
   <si>
+    <t>6 MPE ovitih v prozorno folijo</t>
+  </si>
+  <si>
     <t>temna steklenička s pokrovčkom v kartonski zloženki</t>
   </si>
   <si>
-    <t>6 MPE ovitih v prozorno folijo</t>
-  </si>
-  <si>
-    <t>57x57x131</t>
-  </si>
-  <si>
-    <t>195x130x150</t>
-  </si>
-  <si>
     <t>1188</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>V temnem in suhem prostoru pri temperaturi 18-25 °C obrnjen s pokrovčkom navzgor.</t>
-  </si>
-  <si>
-    <t>Zaščiteno pred vlago in mehanskimi poškodbami. Tovor je potrebno zaščititi pred drsenjem, udarci in prevračanjem.</t>
-  </si>
-  <si>
-    <t>61001</t>
+    <t>40408</t>
+  </si>
+  <si>
+    <t>BIO keksi pomaranča 150 g</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
+  </si>
+  <si>
+    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
+  </si>
+  <si>
+    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
+  </si>
+  <si>
+    <t>1861</t>
+  </si>
+  <si>
+    <t>kJ</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
+    <t>kcal</t>
+  </si>
+  <si>
+    <t>16,6</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>63,5</t>
+  </si>
+  <si>
+    <t>21,7</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>8,1</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>110x400x190</t>
+  </si>
+  <si>
+    <t>110x40x190</t>
+  </si>
+  <si>
+    <t>V suhem prostoru.</t>
+  </si>
+  <si>
+    <t>150 g</t>
+  </si>
+  <si>
+    <t>15 mesecev</t>
+  </si>
+  <si>
+    <t>Kartonska škatla</t>
+  </si>
+  <si>
+    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
+  </si>
+  <si>
+    <t>1920</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
   <si>
     <t>32306</t>
@@ -442,31 +518,112 @@
     <t>≤ 9,0 %</t>
   </si>
   <si>
-    <t>150 g</t>
+    <t>290x145x230</t>
+  </si>
+  <si>
+    <t>55x55x105</t>
+  </si>
+  <si>
+    <t>V temnem in suhem prostoru pri temperaturi 15-25 °C.</t>
+  </si>
+  <si>
+    <t>18 mesecev</t>
+  </si>
+  <si>
+    <t>6 MPE kartonasti zbirni zloženki</t>
   </si>
   <si>
     <t>Vrečke z zip zapiranjem</t>
   </si>
   <si>
-    <t>55x55x105</t>
-  </si>
-  <si>
-    <t>6 MPE kartonasti zbirni zloženki</t>
-  </si>
-  <si>
     <t>600</t>
   </si>
   <si>
-    <t>290x145x230</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>V temnem in suhem prostoru pri temperaturi 15-25 °C.</t>
-  </si>
-  <si>
-    <t>18 mesecev</t>
+    <t>32333</t>
+  </si>
+  <si>
+    <t>KOLAGENBODY 150 G</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
+  </si>
+  <si>
+    <t>Bel prah/granule</t>
+  </si>
+  <si>
+    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
+  </si>
+  <si>
+    <t>&lt; 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cfu/g</t>
+  </si>
+  <si>
+    <t>/1 g</t>
+  </si>
+  <si>
+    <t>&lt; 10</t>
+  </si>
+  <si>
+    <t>max. 8 %</t>
+  </si>
+  <si>
+    <t>min. 0,8 %</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>364</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>1875</t>
+  </si>
+  <si>
+    <t>245x165x115</t>
+  </si>
+  <si>
+    <t>80x80x115</t>
+  </si>
+  <si>
+    <t>36 mesecev</t>
+  </si>
+  <si>
+    <t>pločevinka</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>30140</t>
@@ -493,21 +650,12 @@
     <t>1429</t>
   </si>
   <si>
-    <t>kJ</t>
-  </si>
-  <si>
     <t>336</t>
   </si>
   <si>
-    <t>kcal</t>
-  </si>
-  <si>
     <t>0,4</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>83</t>
   </si>
   <si>
@@ -517,175 +665,25 @@
     <t>0,018</t>
   </si>
   <si>
+    <t>192x138x87</t>
+  </si>
+  <si>
+    <t>62x65x85</t>
+  </si>
+  <si>
+    <t>V temnem, suhem prostoru pri sobni temperaturi obrnjen s pokrovom navzgor.</t>
+  </si>
+  <si>
     <t>250 g</t>
   </si>
   <si>
+    <t>6 MPE v kartonskem podstavku povitih s folijo</t>
+  </si>
+  <si>
     <t>Steklen kozarec s kovinskim pokrovčkom</t>
   </si>
   <si>
-    <t>6 MPE v kartonskem podstavku povitih s folijo</t>
-  </si>
-  <si>
-    <t>62x65x85</t>
-  </si>
-  <si>
-    <t>192x138x87</t>
-  </si>
-  <si>
     <t>1392</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>V temnem, suhem prostoru pri sobni temperaturi obrnjen s pokrovom navzgor.</t>
-  </si>
-  <si>
-    <t>40408</t>
-  </si>
-  <si>
-    <t>BIO keksi pomaranča 150 g</t>
-  </si>
-  <si>
-    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
-  </si>
-  <si>
-    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
-  </si>
-  <si>
-    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
-  </si>
-  <si>
-    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
-  </si>
-  <si>
-    <t>1861</t>
-  </si>
-  <si>
-    <t>445</t>
-  </si>
-  <si>
-    <t>16,6</t>
-  </si>
-  <si>
-    <t>3,6</t>
-  </si>
-  <si>
-    <t>63,5</t>
-  </si>
-  <si>
-    <t>21,7</t>
-  </si>
-  <si>
-    <t>8,1</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>7,7</t>
-  </si>
-  <si>
-    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
-  </si>
-  <si>
-    <t>Kartonska škatla</t>
-  </si>
-  <si>
-    <t>110x40x190</t>
-  </si>
-  <si>
-    <t>110x400x190</t>
-  </si>
-  <si>
-    <t>1920</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>V suhem prostoru.</t>
-  </si>
-  <si>
-    <t>15 mesecev</t>
-  </si>
-  <si>
-    <t>32333</t>
-  </si>
-  <si>
-    <t>KOLAGENBODY 150 G</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
-  </si>
-  <si>
-    <t>Bel prah/granule</t>
-  </si>
-  <si>
-    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
-  </si>
-  <si>
-    <t>&lt; 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cfu/g</t>
-  </si>
-  <si>
-    <t>/1 g</t>
-  </si>
-  <si>
-    <t>&lt; 10</t>
-  </si>
-  <si>
-    <t>max. 8 %</t>
-  </si>
-  <si>
-    <t>min. 0,8 %</t>
-  </si>
-  <si>
-    <t>1523</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>0,6</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>2,7</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>1875</t>
-  </si>
-  <si>
-    <t>pločevinka</t>
-  </si>
-  <si>
-    <t>80x80x115</t>
-  </si>
-  <si>
-    <t>1008</t>
-  </si>
-  <si>
-    <t>245x165x115</t>
-  </si>
-  <si>
-    <t>36 mesecev</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BZ8"/>
+  <dimension ref="A1:BZ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1396,34 +1394,34 @@
       <c r="BM2" t="s"/>
       <c r="BN2" t="s"/>
       <c r="BO2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP2" t="s">
         <v>97</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>98</v>
       </c>
       <c r="BQ2" t="s">
         <v>80</v>
       </c>
       <c r="BR2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BS2" t="s">
         <v>99</v>
       </c>
-      <c r="BS2" t="s">
-        <v>80</v>
-      </c>
       <c r="BT2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="BU2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BV2" t="s">
         <v>80</v>
       </c>
       <c r="BW2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="BX2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="BY2" t="s">
         <v>103</v>
@@ -1560,37 +1558,37 @@
       <c r="BM3" t="s"/>
       <c r="BN3" t="s"/>
       <c r="BO3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP3" t="s">
         <v>123</v>
       </c>
-      <c r="BP3" t="s">
+      <c r="BQ3" t="s">
         <v>124</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="BR3" t="s">
         <v>125</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="BS3" t="s">
         <v>126</v>
       </c>
-      <c r="BS3" t="s">
+      <c r="BT3" t="s">
         <v>127</v>
       </c>
-      <c r="BT3" t="s">
-        <v>125</v>
-      </c>
       <c r="BU3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BV3" t="s">
         <v>128</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>80</v>
       </c>
       <c r="BW3" t="s">
         <v>129</v>
       </c>
       <c r="BX3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BY3" t="s">
         <v>130</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>103</v>
       </c>
       <c r="BZ3" t="s">
         <v>131</v>
@@ -1600,14 +1598,24 @@
       <c r="A4" t="s">
         <v>132</v>
       </c>
-      <c r="B4" t="s"/>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
       <c r="C4" t="s">
         <v>80</v>
       </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s"/>
-      <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
       <c r="H4" t="s"/>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
@@ -1633,24 +1641,60 @@
       <c r="AD4" t="s"/>
       <c r="AE4" t="s"/>
       <c r="AF4" t="s"/>
-      <c r="AG4" t="s"/>
-      <c r="AH4" t="s"/>
-      <c r="AI4" t="s"/>
-      <c r="AJ4" t="s"/>
-      <c r="AK4" t="s"/>
-      <c r="AL4" t="s"/>
-      <c r="AM4" t="s"/>
-      <c r="AN4" t="s"/>
-      <c r="AO4" t="s"/>
-      <c r="AP4" t="s"/>
-      <c r="AQ4" t="s"/>
-      <c r="AR4" t="s"/>
-      <c r="AS4" t="s"/>
-      <c r="AT4" t="s"/>
-      <c r="AU4" t="s"/>
-      <c r="AV4" t="s"/>
-      <c r="AW4" t="s"/>
-      <c r="AX4" t="s"/>
+      <c r="AG4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>119</v>
+      </c>
       <c r="AY4" t="s"/>
       <c r="AZ4" t="s"/>
       <c r="BA4" t="s"/>
@@ -1667,43 +1711,65 @@
       <c r="BL4" t="s"/>
       <c r="BM4" t="s"/>
       <c r="BN4" t="s"/>
-      <c r="BO4" t="s"/>
-      <c r="BP4" t="s"/>
-      <c r="BQ4" t="s"/>
-      <c r="BR4" t="s"/>
+      <c r="BO4" t="s">
+        <v>149</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>149</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>151</v>
+      </c>
       <c r="BS4" t="s"/>
-      <c r="BT4" t="s"/>
-      <c r="BU4" t="s"/>
-      <c r="BV4" t="s"/>
-      <c r="BW4" t="s"/>
-      <c r="BX4" t="s"/>
-      <c r="BY4" t="s"/>
-      <c r="BZ4" t="s"/>
+      <c r="BT4" t="s">
+        <v>152</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>153</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>154</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>156</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:78">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H5" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="I5" t="s">
         <v>89</v>
@@ -1718,7 +1784,7 @@
         <v>111</v>
       </c>
       <c r="M5" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="N5" t="s">
         <v>113</v>
@@ -1752,7 +1818,7 @@
       <c r="AC5" t="s"/>
       <c r="AD5" t="s"/>
       <c r="AE5" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="AF5" t="s"/>
       <c r="AG5" t="s"/>
@@ -1790,79 +1856,71 @@
       <c r="BM5" t="s"/>
       <c r="BN5" t="s"/>
       <c r="BO5" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="BP5" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="BQ5" t="s">
         <v>80</v>
       </c>
       <c r="BR5" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="BS5" t="s">
+        <v>126</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>152</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>170</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>171</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>172</v>
+      </c>
+      <c r="BX5" t="s">
         <v>80</v>
       </c>
-      <c r="BT5" t="s">
-        <v>145</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>146</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>147</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>148</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>149</v>
-      </c>
       <c r="BY5" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="BZ5" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:78">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="G6" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" t="s">
-        <v>111</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I6" t="s"/>
+      <c r="J6" t="s"/>
+      <c r="K6" t="s"/>
+      <c r="L6" t="s"/>
       <c r="M6" t="s"/>
       <c r="N6" t="s"/>
       <c r="O6" t="s">
@@ -1871,19 +1929,23 @@
       <c r="P6" t="s">
         <v>90</v>
       </c>
-      <c r="Q6" t="s"/>
-      <c r="R6" t="s"/>
+      <c r="Q6" t="s">
+        <v>181</v>
+      </c>
+      <c r="R6" t="s">
+        <v>182</v>
+      </c>
       <c r="S6" t="s">
         <v>89</v>
       </c>
       <c r="T6" t="s">
-        <v>111</v>
+        <v>183</v>
       </c>
       <c r="U6" t="s">
-        <v>89</v>
+        <v>184</v>
       </c>
       <c r="V6" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="W6" t="s"/>
       <c r="X6" t="s"/>
@@ -1891,64 +1953,72 @@
         <v>112</v>
       </c>
       <c r="Z6" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="AA6" t="s"/>
       <c r="AB6" t="s"/>
       <c r="AC6" t="s"/>
       <c r="AD6" t="s"/>
-      <c r="AE6" t="s"/>
-      <c r="AF6" t="s"/>
+      <c r="AE6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>186</v>
+      </c>
       <c r="AG6" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="AH6" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="AI6" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="AJ6" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="AK6" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="AL6" t="s">
         <v>119</v>
       </c>
       <c r="AM6" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="AN6" t="s">
         <v>119</v>
       </c>
       <c r="AO6" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="AP6" t="s">
         <v>119</v>
       </c>
       <c r="AQ6" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="AR6" t="s">
         <v>119</v>
       </c>
       <c r="AS6" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="AT6" t="s">
         <v>119</v>
       </c>
       <c r="AU6" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="AV6" t="s">
         <v>119</v>
       </c>
-      <c r="AW6" t="s"/>
-      <c r="AX6" t="s"/>
+      <c r="AW6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>119</v>
+      </c>
       <c r="AY6" t="s"/>
       <c r="AZ6" t="s"/>
       <c r="BA6" t="s"/>
@@ -1957,148 +2027,182 @@
       <c r="BD6" t="s"/>
       <c r="BE6" t="s"/>
       <c r="BF6" t="s"/>
-      <c r="BG6" t="s"/>
-      <c r="BH6" t="s"/>
+      <c r="BG6" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>95</v>
+      </c>
       <c r="BI6" t="s"/>
       <c r="BJ6" t="s"/>
-      <c r="BK6" t="s"/>
-      <c r="BL6" t="s"/>
-      <c r="BM6" t="s"/>
-      <c r="BN6" t="s"/>
+      <c r="BK6" t="s">
+        <v>195</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>196</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>95</v>
+      </c>
       <c r="BO6" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="BP6" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="BQ6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR6" t="s">
         <v>169</v>
       </c>
-      <c r="BR6" t="s">
-        <v>170</v>
-      </c>
       <c r="BS6" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="BT6" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="BU6" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="BV6" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="BW6" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="BX6" t="s">
-        <v>174</v>
+        <v>80</v>
       </c>
       <c r="BY6" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="BZ6" t="s">
-        <v>131</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:78">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="E7" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F7" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="G7" t="s">
-        <v>180</v>
-      </c>
-      <c r="H7" t="s"/>
-      <c r="I7" t="s"/>
-      <c r="J7" t="s"/>
-      <c r="K7" t="s"/>
-      <c r="L7" t="s"/>
+        <v>208</v>
+      </c>
+      <c r="H7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" t="s">
+        <v>111</v>
+      </c>
       <c r="M7" t="s"/>
       <c r="N7" t="s"/>
-      <c r="O7" t="s"/>
-      <c r="P7" t="s"/>
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" t="s">
+        <v>90</v>
+      </c>
       <c r="Q7" t="s"/>
       <c r="R7" t="s"/>
-      <c r="S7" t="s"/>
-      <c r="T7" t="s"/>
-      <c r="U7" t="s"/>
-      <c r="V7" t="s"/>
+      <c r="S7" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" t="s">
+        <v>111</v>
+      </c>
+      <c r="U7" t="s">
+        <v>89</v>
+      </c>
+      <c r="V7" t="s">
+        <v>114</v>
+      </c>
       <c r="W7" t="s"/>
       <c r="X7" t="s"/>
       <c r="Y7" t="s"/>
       <c r="Z7" t="s"/>
-      <c r="AA7" t="s"/>
-      <c r="AB7" t="s"/>
+      <c r="AA7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>113</v>
+      </c>
       <c r="AC7" t="s"/>
       <c r="AD7" t="s"/>
       <c r="AE7" t="s"/>
       <c r="AF7" t="s"/>
       <c r="AG7" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="AH7" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="AI7" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="AJ7" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="AK7" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="AL7" t="s">
         <v>119</v>
       </c>
       <c r="AM7" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="AN7" t="s">
         <v>119</v>
       </c>
       <c r="AO7" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="AP7" t="s">
         <v>119</v>
       </c>
       <c r="AQ7" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="AR7" t="s">
         <v>119</v>
       </c>
-      <c r="AS7" t="s">
-        <v>187</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>119</v>
-      </c>
+      <c r="AS7" t="s"/>
+      <c r="AT7" t="s"/>
       <c r="AU7" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="AV7" t="s">
         <v>119</v>
       </c>
       <c r="AW7" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="AX7" t="s">
         <v>119</v>
@@ -2120,230 +2224,40 @@
       <c r="BM7" t="s"/>
       <c r="BN7" t="s"/>
       <c r="BO7" t="s">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="BP7" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="BQ7" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="BR7" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="BS7" t="s">
-        <v>193</v>
+        <v>126</v>
       </c>
       <c r="BT7" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="BU7" t="s">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="BV7" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="BW7" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="BX7" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="BY7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BZ7" t="s"/>
-    </row>
-    <row r="8" spans="1:78">
-      <c r="A8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" t="s">
+        <v>222</v>
+      </c>
+      <c r="BZ7" t="s">
         <v>202</v>
-      </c>
-      <c r="G8" t="s">
-        <v>203</v>
-      </c>
-      <c r="H8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I8" t="s"/>
-      <c r="J8" t="s"/>
-      <c r="K8" t="s"/>
-      <c r="L8" t="s"/>
-      <c r="M8" t="s"/>
-      <c r="N8" t="s"/>
-      <c r="O8" t="s">
-        <v>89</v>
-      </c>
-      <c r="P8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>204</v>
-      </c>
-      <c r="R8" t="s">
-        <v>205</v>
-      </c>
-      <c r="S8" t="s">
-        <v>89</v>
-      </c>
-      <c r="T8" t="s">
-        <v>206</v>
-      </c>
-      <c r="U8" t="s">
-        <v>207</v>
-      </c>
-      <c r="V8" t="s">
-        <v>205</v>
-      </c>
-      <c r="W8" t="s"/>
-      <c r="X8" t="s"/>
-      <c r="Y8" t="s"/>
-      <c r="Z8" t="s"/>
-      <c r="AA8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>205</v>
-      </c>
-      <c r="AC8" t="s"/>
-      <c r="AD8" t="s"/>
-      <c r="AE8" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>209</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>211</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>161</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>212</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>213</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>214</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>213</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AY8" t="s"/>
-      <c r="AZ8" t="s"/>
-      <c r="BA8" t="s"/>
-      <c r="BB8" t="s"/>
-      <c r="BC8" t="s"/>
-      <c r="BD8" t="s"/>
-      <c r="BE8" t="s"/>
-      <c r="BF8" t="s"/>
-      <c r="BG8" t="s">
-        <v>216</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>95</v>
-      </c>
-      <c r="BI8" t="s"/>
-      <c r="BJ8" t="s"/>
-      <c r="BK8" t="s">
-        <v>217</v>
-      </c>
-      <c r="BL8" t="s">
-        <v>119</v>
-      </c>
-      <c r="BM8" t="s">
-        <v>218</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>95</v>
-      </c>
-      <c r="BO8" t="s">
-        <v>142</v>
-      </c>
-      <c r="BP8" t="s">
-        <v>219</v>
-      </c>
-      <c r="BQ8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BR8" t="s">
-        <v>220</v>
-      </c>
-      <c r="BS8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>125</v>
-      </c>
-      <c r="BU8" t="s">
-        <v>221</v>
-      </c>
-      <c r="BV8" t="s">
-        <v>222</v>
-      </c>
-      <c r="BW8" t="s">
-        <v>173</v>
-      </c>
-      <c r="BX8" t="s">
-        <v>149</v>
-      </c>
-      <c r="BY8" t="s">
-        <v>223</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aktivne,mikrobiološke,mašboe,energijska vrednost. Header format
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="192">
   <si>
     <t>Šifra</t>
   </si>
@@ -40,49 +40,49 @@
     <t>Zakonodaja</t>
   </si>
   <si>
-    <t>Bacillus cereus /0,01g</t>
-  </si>
-  <si>
-    <t>Bacillus cereus /g</t>
-  </si>
-  <si>
-    <t>Escherichia coli /0,01g</t>
-  </si>
-  <si>
-    <t>Escherichia coli /g</t>
-  </si>
-  <si>
-    <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus /0,01g</t>
-  </si>
-  <si>
-    <t>Kvasovke in plesni /g</t>
-  </si>
-  <si>
-    <t>Plesni in kvasovke /g</t>
-  </si>
-  <si>
-    <t>Salmonella /25g</t>
-  </si>
-  <si>
-    <t>Skupno število /g</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus /0,01g</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus /g</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji /0,1g</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus /1g</t>
-  </si>
-  <si>
-    <t>Enterobakterije /g</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji /g</t>
+    <t>Bacillus cereus (/0,01g)</t>
+  </si>
+  <si>
+    <t>Bacillus cereus (/g)</t>
+  </si>
+  <si>
+    <t>Escherichia coli (/0,01g)</t>
+  </si>
+  <si>
+    <t>Escherichia coli (/g)</t>
+  </si>
+  <si>
+    <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus (/0,01g)</t>
+  </si>
+  <si>
+    <t>Kvasovke in plesni (/g)</t>
+  </si>
+  <si>
+    <t>Plesni in kvasovke (/g)</t>
+  </si>
+  <si>
+    <t>Salmonella (/25g)</t>
+  </si>
+  <si>
+    <t>Skupno število (/g)</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus (/0,01g)</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus (/g)</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji (/0,1g)</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus (/1g)</t>
+  </si>
+  <si>
+    <t>Enterobakterije (/g)</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji (/g)</t>
   </si>
   <si>
     <t>Gostota</t>
@@ -97,28 +97,16 @@
     <t>Vitamin C</t>
   </si>
   <si>
-    <t>Energijska vrednost 1</t>
-  </si>
-  <si>
-    <t>ENV1 Enote</t>
-  </si>
-  <si>
-    <t>Energijska vrednost 2</t>
-  </si>
-  <si>
-    <t>ENV2 Enote</t>
-  </si>
-  <si>
-    <t>Maščobe</t>
-  </si>
-  <si>
-    <t>M Enote</t>
-  </si>
-  <si>
-    <t>Nasičene</t>
-  </si>
-  <si>
-    <t>MN Enote</t>
+    <t>Energijska vrednost (kJ)</t>
+  </si>
+  <si>
+    <t>Energijska vrednost (kcal)</t>
+  </si>
+  <si>
+    <t>Maščobe (g)</t>
+  </si>
+  <si>
+    <t>Nasičene M. (g)</t>
   </si>
   <si>
     <t>Ogljikovi hidrati</t>
@@ -151,28 +139,28 @@
     <t>PV Enote</t>
   </si>
   <si>
-    <t>Izvleček smrekovih vršičkov(akt) mg</t>
-  </si>
-  <si>
-    <t>Kofein iz gvarane(akt) mg</t>
-  </si>
-  <si>
-    <t>Med(akt) g</t>
-  </si>
-  <si>
-    <t>Vitamin A(akt) μg</t>
-  </si>
-  <si>
-    <t>Vitamin C(akt) mg</t>
-  </si>
-  <si>
-    <t>niacin(akt) mg</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance®(akt) g</t>
-  </si>
-  <si>
-    <t>Magnezij(akt) mg</t>
+    <t>Izvleček smrekovih vršičkov(akt) (mg)</t>
+  </si>
+  <si>
+    <t>Kofein iz gvarane(akt) (mg)</t>
+  </si>
+  <si>
+    <t>Med(akt) (g)</t>
+  </si>
+  <si>
+    <t>Vitamin A(akt) (μg)</t>
+  </si>
+  <si>
+    <t>Vitamin C(akt) (mg)</t>
+  </si>
+  <si>
+    <t>niacin(akt) (mg)</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance®(akt) (g)</t>
+  </si>
+  <si>
+    <t>Magnezij(akt) (mg)</t>
   </si>
   <si>
     <t>dimenzija KP</t>
@@ -424,22 +412,16 @@
     <t>1429</t>
   </si>
   <si>
-    <t>kJ</t>
-  </si>
-  <si>
     <t>336</t>
   </si>
   <si>
-    <t>kcal</t>
-  </si>
-  <si>
     <t>0,4</t>
   </si>
   <si>
+    <t>83</t>
+  </si>
+  <si>
     <t>g</t>
-  </si>
-  <si>
-    <t>83</t>
   </si>
   <si>
     <t>0,2</t>
@@ -956,7 +938,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM7"/>
+  <dimension ref="A1:BI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -964,7 +946,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:61">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,73 +1130,61 @@
       <c r="BI1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:61">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:65">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
-        <v>72</v>
       </c>
       <c r="I2" t="s"/>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s"/>
       <c r="N2" t="s"/>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R2" t="s"/>
       <c r="S2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="T2" t="s"/>
       <c r="U2" t="s"/>
       <c r="V2" t="s"/>
       <c r="W2" t="s"/>
       <c r="X2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Y2" t="s"/>
       <c r="Z2" t="s"/>
@@ -1234,115 +1204,111 @@
       <c r="AN2" t="s"/>
       <c r="AO2" t="s"/>
       <c r="AP2" t="s"/>
-      <c r="AQ2" t="s"/>
+      <c r="AQ2" t="s">
+        <v>74</v>
+      </c>
       <c r="AR2" t="s"/>
       <c r="AS2" t="s"/>
       <c r="AT2" t="s"/>
       <c r="AU2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AV2" t="s"/>
       <c r="AW2" t="s"/>
-      <c r="AX2" t="s"/>
+      <c r="AX2" t="s">
+        <v>63</v>
+      </c>
       <c r="AY2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC2" t="s">
         <v>79</v>
       </c>
-      <c r="AZ2" t="s"/>
-      <c r="BA2" t="s"/>
-      <c r="BB2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>80</v>
       </c>
-      <c r="BD2" t="s">
-        <v>67</v>
-      </c>
       <c r="BE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF2" t="s">
         <v>81</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH2" t="s">
         <v>82</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
         <v>83</v>
       </c>
-      <c r="BH2" t="s">
+    </row>
+    <row r="3" spans="1:61">
+      <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="BI2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BJ2" t="s">
+      <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="BK2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
         <v>86</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="E3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:65">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" t="s">
-        <v>93</v>
-      </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s"/>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L3" t="s"/>
       <c r="M3" t="s"/>
       <c r="N3" t="s"/>
       <c r="O3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q3" t="s"/>
       <c r="R3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="S3" t="s"/>
       <c r="T3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s"/>
       <c r="W3" t="s"/>
       <c r="X3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Y3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Z3" t="s"/>
       <c r="AA3" t="s"/>
@@ -1360,111 +1326,107 @@
       <c r="AM3" t="s"/>
       <c r="AN3" t="s"/>
       <c r="AO3" t="s"/>
-      <c r="AP3" t="s"/>
+      <c r="AP3" t="s">
+        <v>93</v>
+      </c>
       <c r="AQ3" t="s"/>
-      <c r="AR3" t="s"/>
-      <c r="AS3" t="s"/>
+      <c r="AR3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>95</v>
+      </c>
       <c r="AT3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU3" t="s"/>
+      <c r="AV3" t="s"/>
+      <c r="AW3" t="s"/>
+      <c r="AX3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY3" t="s">
         <v>97</v>
       </c>
-      <c r="AU3" t="s"/>
-      <c r="AV3" t="s">
+      <c r="AZ3" t="s">
         <v>98</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="BA3" t="s">
         <v>99</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="BB3" t="s">
         <v>100</v>
-      </c>
-      <c r="AY3" t="s"/>
-      <c r="AZ3" t="s"/>
-      <c r="BA3" t="s"/>
-      <c r="BB3" t="s">
-        <v>67</v>
       </c>
       <c r="BC3" t="s">
         <v>101</v>
       </c>
       <c r="BD3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE3" t="s">
         <v>102</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>103</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BH3" t="s">
         <v>104</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BI3" t="s">
         <v>105</v>
       </c>
-      <c r="BH3" t="s">
-        <v>84</v>
-      </c>
-      <c r="BI3" t="s">
+    </row>
+    <row r="4" spans="1:61">
+      <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="BJ3" t="s">
+      <c r="B4" t="s">
         <v>107</v>
       </c>
-      <c r="BK3" t="s">
-        <v>106</v>
-      </c>
-      <c r="BL3" t="s">
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="E4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:65">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>112</v>
       </c>
-      <c r="E4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" t="s">
-        <v>116</v>
-      </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s"/>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L4" t="s"/>
       <c r="M4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N4" t="s"/>
       <c r="O4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q4" t="s"/>
       <c r="R4" t="s"/>
       <c r="S4" t="s"/>
       <c r="T4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="U4" t="s"/>
       <c r="V4" t="s"/>
@@ -1472,7 +1434,7 @@
       <c r="X4" t="s"/>
       <c r="Y4" t="s"/>
       <c r="Z4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AA4" t="s"/>
       <c r="AB4" t="s"/>
@@ -1497,95 +1459,91 @@
       <c r="AU4" t="s"/>
       <c r="AV4" t="s"/>
       <c r="AW4" t="s"/>
-      <c r="AX4" t="s"/>
-      <c r="AY4" t="s"/>
-      <c r="AZ4" t="s"/>
-      <c r="BA4" t="s"/>
+      <c r="AX4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>117</v>
+      </c>
       <c r="BB4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD4" t="s">
         <v>119</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BE4" t="s">
         <v>120</v>
       </c>
-      <c r="BD4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE4" t="s">
+      <c r="BF4" t="s">
         <v>121</v>
       </c>
-      <c r="BF4" t="s">
-        <v>104</v>
-      </c>
       <c r="BG4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH4" t="s">
         <v>122</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BI4" t="s">
         <v>123</v>
       </c>
-      <c r="BI4" t="s">
+    </row>
+    <row r="5" spans="1:61">
+      <c r="A5" t="s">
         <v>124</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="B5" t="s">
         <v>125</v>
       </c>
-      <c r="BK4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL4" t="s">
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
         <v>126</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="E5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:65">
-      <c r="A5" t="s">
+      <c r="F5" t="s">
         <v>128</v>
       </c>
-      <c r="B5" t="s">
+      <c r="G5" t="s">
         <v>129</v>
       </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>130</v>
       </c>
-      <c r="E5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" t="s">
-        <v>134</v>
-      </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s"/>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s"/>
       <c r="M5" t="s"/>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s"/>
       <c r="P5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q5" t="s"/>
       <c r="R5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="S5" t="s"/>
       <c r="T5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="U5" t="s"/>
       <c r="V5" t="s"/>
@@ -1595,121 +1553,109 @@
       <c r="Z5" t="s"/>
       <c r="AA5" t="s"/>
       <c r="AB5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG5" t="s">
         <v>135</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AH5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>136</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AK5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL5" t="s">
         <v>137</v>
       </c>
-      <c r="AE5" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>139</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>141</v>
-      </c>
       <c r="AM5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>142</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>143</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>140</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="AN5" t="s"/>
+      <c r="AO5" t="s"/>
+      <c r="AP5" t="s"/>
+      <c r="AQ5" t="s"/>
       <c r="AR5" t="s"/>
       <c r="AS5" t="s"/>
       <c r="AT5" t="s"/>
       <c r="AU5" t="s"/>
       <c r="AV5" t="s"/>
       <c r="AW5" t="s"/>
-      <c r="AX5" t="s"/>
-      <c r="AY5" t="s"/>
-      <c r="AZ5" t="s"/>
-      <c r="BA5" t="s"/>
+      <c r="AX5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>138</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>140</v>
+      </c>
       <c r="BB5" t="s">
+        <v>100</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>142</v>
+      </c>
+      <c r="BH5" t="s">
         <v>144</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BI5" t="s">
         <v>145</v>
       </c>
-      <c r="BD5" t="s">
-        <v>144</v>
-      </c>
-      <c r="BE5" t="s">
+    </row>
+    <row r="6" spans="1:61">
+      <c r="A6" t="s">
         <v>146</v>
       </c>
-      <c r="BF5" t="s">
-        <v>104</v>
-      </c>
-      <c r="BG5" t="s">
+      <c r="B6" t="s">
         <v>147</v>
       </c>
-      <c r="BH5" t="s">
-        <v>84</v>
-      </c>
-      <c r="BI5" t="s">
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
         <v>148</v>
       </c>
-      <c r="BJ5" t="s">
+      <c r="E6" t="s">
         <v>149</v>
       </c>
-      <c r="BK5" t="s">
-        <v>148</v>
-      </c>
-      <c r="BL5" t="s">
+      <c r="F6" t="s">
         <v>150</v>
       </c>
-      <c r="BM5" t="s">
+      <c r="G6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:65">
-      <c r="A6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6" t="s">
-        <v>157</v>
       </c>
       <c r="H6" t="s"/>
       <c r="I6" t="s"/>
@@ -1732,126 +1678,114 @@
       <c r="Z6" t="s"/>
       <c r="AA6" t="s"/>
       <c r="AB6" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>158</v>
       </c>
-      <c r="AC6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD6" t="s">
+      <c r="AK6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL6" t="s">
         <v>159</v>
       </c>
-      <c r="AE6" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="AM6" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN6" t="s">
         <v>160</v>
       </c>
-      <c r="AG6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>161</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>163</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>164</v>
-      </c>
       <c r="AO6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>165</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>166</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>140</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="AP6" t="s"/>
+      <c r="AQ6" t="s"/>
+      <c r="AR6" t="s"/>
+      <c r="AS6" t="s"/>
       <c r="AT6" t="s"/>
       <c r="AU6" t="s"/>
       <c r="AV6" t="s"/>
       <c r="AW6" t="s"/>
-      <c r="AX6" t="s"/>
-      <c r="AY6" t="s"/>
-      <c r="AZ6" t="s"/>
-      <c r="BA6" t="s"/>
-      <c r="BB6" t="s">
+      <c r="AX6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>162</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>161</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB6" t="s"/>
+      <c r="BC6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>164</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>166</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>165</v>
+      </c>
+      <c r="BH6" t="s">
         <v>167</v>
       </c>
-      <c r="BC6" t="s">
+      <c r="BI6" t="s">
         <v>168</v>
       </c>
-      <c r="BD6" t="s">
-        <v>167</v>
-      </c>
-      <c r="BE6" t="s">
+    </row>
+    <row r="7" spans="1:61">
+      <c r="A7" t="s">
         <v>169</v>
       </c>
-      <c r="BF6" t="s"/>
-      <c r="BG6" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH6" t="s">
+      <c r="B7" t="s">
         <v>170</v>
       </c>
-      <c r="BI6" t="s">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
         <v>171</v>
       </c>
-      <c r="BJ6" t="s">
+      <c r="E7" t="s">
         <v>172</v>
       </c>
-      <c r="BK6" t="s">
-        <v>171</v>
-      </c>
-      <c r="BL6" t="s">
+      <c r="F7" t="s">
         <v>173</v>
       </c>
-      <c r="BM6" t="s">
+      <c r="G7" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="1:65">
-      <c r="A7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G7" t="s">
-        <v>180</v>
-      </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s"/>
       <c r="J7" t="s"/>
@@ -1861,134 +1795,122 @@
       <c r="N7" t="s"/>
       <c r="O7" t="s"/>
       <c r="P7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="R7" t="s"/>
       <c r="S7" t="s"/>
       <c r="T7" t="s"/>
       <c r="U7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="V7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="W7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="X7" t="s"/>
       <c r="Y7" t="s"/>
       <c r="Z7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>180</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>182</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AK7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN7" t="s">
         <v>183</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AO7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP7" t="s"/>
+      <c r="AQ7" t="s"/>
+      <c r="AR7" t="s"/>
+      <c r="AS7" t="s"/>
+      <c r="AT7" t="s">
         <v>184</v>
       </c>
-      <c r="AC7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD7" t="s">
+      <c r="AU7" t="s"/>
+      <c r="AV7" t="s">
         <v>185</v>
       </c>
-      <c r="AE7" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ7" t="s">
+      <c r="AW7" t="s">
         <v>186</v>
       </c>
-      <c r="AK7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL7" t="s">
+      <c r="AX7" t="s">
         <v>187</v>
       </c>
-      <c r="AM7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AN7" t="s">
+      <c r="AY7" t="s">
         <v>188</v>
       </c>
-      <c r="AO7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>187</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR7" t="s">
+      <c r="AZ7" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>100</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD7" t="s">
         <v>189</v>
       </c>
-      <c r="AS7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AT7" t="s"/>
-      <c r="AU7" t="s"/>
-      <c r="AV7" t="s"/>
-      <c r="AW7" t="s"/>
-      <c r="AX7" t="s">
+      <c r="BE7" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF7" t="s">
         <v>190</v>
       </c>
-      <c r="AY7" t="s"/>
-      <c r="AZ7" t="s">
+      <c r="BG7" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH7" t="s">
         <v>191</v>
       </c>
-      <c r="BA7" t="s">
-        <v>192</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>193</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>194</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>121</v>
-      </c>
-      <c r="BF7" t="s">
-        <v>104</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH7" t="s">
-        <v>195</v>
-      </c>
       <c r="BI7" t="s">
-        <v>106</v>
-      </c>
-      <c r="BJ7" t="s">
-        <v>196</v>
-      </c>
-      <c r="BK7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL7" t="s">
-        <v>197</v>
-      </c>
-      <c r="BM7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started a second solution
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="217">
   <si>
     <t>Šifra</t>
   </si>
@@ -52,66 +52,69 @@
     <t>Escherichia coli (/g)</t>
   </si>
   <si>
+    <t>Plesni in kvasovke (/g)</t>
+  </si>
+  <si>
+    <t>Salmonella (/25g)</t>
+  </si>
+  <si>
+    <t>Skupni število (/g)</t>
+  </si>
+  <si>
+    <t>Skupno število (/g)</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus (/0,01g)</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus (/g)</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji (/0,1g)</t>
+  </si>
+  <si>
     <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus (/0,01g)</t>
   </si>
   <si>
+    <t>Staphylococcus aureus (/1g)</t>
+  </si>
+  <si>
+    <t>Enterobakterije (/g)</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji (/g)</t>
+  </si>
+  <si>
     <t>Kvasovke in plesni (/g)</t>
   </si>
   <si>
-    <t>Plesni in kvasovke (/g)</t>
-  </si>
-  <si>
-    <t>Salmonella (/25g)</t>
-  </si>
-  <si>
-    <t>Skupno število (/g)</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus (/0,01g)</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus (/g)</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji (/0,1g)</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus (/1g)</t>
-  </si>
-  <si>
-    <t>Enterobakterije (/g)</t>
-  </si>
-  <si>
-    <t>Sulfitreducirajoči klostridiji (/g)</t>
-  </si>
-  <si>
     <t>[average] Gostota (g/ml)</t>
   </si>
   <si>
+    <t>[min] Gostota (g/ml)</t>
+  </si>
+  <si>
+    <t>[max] Gostota (g/ml)</t>
+  </si>
+  <si>
     <t>[average] Suha snov (%)</t>
   </si>
   <si>
+    <t>[min] Suha snov (%)</t>
+  </si>
+  <si>
+    <t>[max] Suha snov (%)</t>
+  </si>
+  <si>
     <t>[average] Vlaga (%)</t>
   </si>
   <si>
-    <t>[max] Gostota (g/ml)</t>
-  </si>
-  <si>
-    <t>[max] Suha snov (%)</t>
+    <t>[min] Vlaga (%)</t>
   </si>
   <si>
     <t>[max] Vlaga (%)</t>
   </si>
   <si>
-    <t>[min] Gostota (g/ml)</t>
-  </si>
-  <si>
-    <t>[min] Suha snov (%)</t>
-  </si>
-  <si>
-    <t>[min] Vlaga (%)</t>
-  </si>
-  <si>
     <t>[average] Vitamin C (%)</t>
   </si>
   <si>
@@ -139,39 +142,33 @@
     <t>Sladkorji (g)</t>
   </si>
   <si>
+    <t>Prehranske vlaknine (g)</t>
+  </si>
+  <si>
     <t>Beljakovine (g)</t>
   </si>
   <si>
     <t>Sol (g)</t>
   </si>
   <si>
-    <t>Prehranske vlaknine (g)</t>
+    <t>[akt] Kofein iz gvarane (mg)</t>
+  </si>
+  <si>
+    <t>[akt] niacin (mg)</t>
+  </si>
+  <si>
+    <t>[akt] Vitamin A (μg)</t>
+  </si>
+  <si>
+    <t>[akt] Vitamin C (mg)</t>
+  </si>
+  <si>
+    <t>[akt] Med (g)</t>
   </si>
   <si>
     <t>[akt] Izvleček smrekovih vršičkov (mg)</t>
   </si>
   <si>
-    <t>[akt] Kofein iz gvarane (mg)</t>
-  </si>
-  <si>
-    <t>[akt] Med (g)</t>
-  </si>
-  <si>
-    <t>[akt] Vitamin A (μg)</t>
-  </si>
-  <si>
-    <t>[akt] Vitamin C (mg)</t>
-  </si>
-  <si>
-    <t>[akt] niacin (mg)</t>
-  </si>
-  <si>
-    <t>[akt] Hidrolizirani kolagen Bodybalance® (g)</t>
-  </si>
-  <si>
-    <t>[akt] Magnezij (mg)</t>
-  </si>
-  <si>
     <t>dimenzija KP</t>
   </si>
   <si>
@@ -211,114 +208,132 @@
     <t>32226</t>
   </si>
   <si>
+    <t>32006</t>
+  </si>
+  <si>
     <t>32348</t>
   </si>
   <si>
+    <t>40408</t>
+  </si>
+  <si>
     <t>32306</t>
   </si>
   <si>
+    <t>32333</t>
+  </si>
+  <si>
     <t>30140</t>
   </si>
   <si>
-    <t>40408</t>
-  </si>
-  <si>
-    <t>32333</t>
-  </si>
-  <si>
     <t>GUARANA NATURAL ENERGY 5 X 9 ml</t>
   </si>
   <si>
+    <t>APIKOMPLEKS 250 G</t>
+  </si>
+  <si>
     <t>SIRUP SMREKOVI VRŠIČKI 200 ML</t>
   </si>
   <si>
+    <t>BIO keksi pomaranča 150 g</t>
+  </si>
+  <si>
     <t>CVETNI PRAH V VREČKI 150 g</t>
   </si>
   <si>
+    <t>KOLAGENBODY 150 G</t>
+  </si>
+  <si>
     <t>MED AKACIJEV S TARTUFI 250 G</t>
   </si>
   <si>
-    <t>BIO keksi pomaranča 150 g</t>
-  </si>
-  <si>
-    <t>KOLAGENBODY 150 G</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
     <t>Naravni kofein iz gvarane in niacin v raztopini</t>
   </si>
   <si>
+    <t>Med s cvetnim prahom, matičnim mlečkom, propolisom, vitaminom C in riboflavinom (vitamin B2)</t>
+  </si>
+  <si>
     <t>Sirup s smrekovimi vršički, medom in vitaminoma A in C</t>
   </si>
   <si>
+    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
+  </si>
+  <si>
     <t>Naravni čebelji pridelek</t>
   </si>
   <si>
+    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
+  </si>
+  <si>
     <t>Akacijev med s tartufi</t>
   </si>
   <si>
-    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
-  </si>
-  <si>
     <t>Voda, trsni sladkor, 10 % izvleček iz semen gvarane v prahu (Paulina cupana), zgoščeni sok aronije, zgoščeni sok borovnice, uprašeni sok acerole (Malpighia glabra), niacin in konzervans: kalijev sorbat.</t>
   </si>
   <si>
+    <t>Med 94 %, cvetni prah 3 %, matični mleček 1,5 %, 70-odstotni izvleček propolisa 1 %, vitamin C in riboflavin (vitamin B2)</t>
+  </si>
+  <si>
     <t>Med, hruškov zgoščeni sok, tekoči izvleček smrekovih vršičkov (Picea abies), tekoči izvleček listov timijana v prahu (Thymus vulgaris), tekoči izvleček listov poprove mete (Mentha x piperita), vitamin C (L-askorbinska kislina), vitamin A (retinil palmitat), olje listov evkaliptusa (Eucalyptus globulus)</t>
   </si>
   <si>
+    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
+  </si>
+  <si>
     <t>Cvetni prah 100 %</t>
   </si>
   <si>
+    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
+  </si>
+  <si>
     <t>Akacijev med 99 %, črni tartufi (Tuber aestivum) 1 %</t>
   </si>
   <si>
-    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
-  </si>
-  <si>
-    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
-  </si>
-  <si>
     <t>Temno vijolična tekočina z usedlino na dnu fiole, brez tujih primesi</t>
   </si>
   <si>
+    <t>oranžno rumena, homogeno kristalizirana masa z rahlo peno na površini</t>
+  </si>
+  <si>
     <t>svetlo rjava, viskozna tekočina</t>
   </si>
   <si>
+    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
+  </si>
+  <si>
     <t>Granule različne barve od rumene, rdeče, rjave do sive, različnih oblik in velikosti</t>
   </si>
   <si>
+    <t>Bel prah/granule</t>
+  </si>
+  <si>
     <t>Gosta, viskozna tekočina rumene barve, z rjavimi, črnimi koščki tartufov na vrhu kozarca</t>
   </si>
   <si>
-    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
-  </si>
-  <si>
-    <t>Bel prah/granule</t>
-  </si>
-  <si>
     <t>Grenko sladkega okusa, aroma po borovnici in gvarani</t>
   </si>
   <si>
+    <t>sladko grenki okus, aroma po medu, propolisu in matičnem mlečku</t>
+  </si>
+  <si>
     <t>sladkega okusa, aroma po medu, timijanu, poprovi meti in evkaliptusu</t>
   </si>
   <si>
+    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
+  </si>
+  <si>
     <t>Grenko sladkega okusa</t>
   </si>
   <si>
+    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
+  </si>
+  <si>
     <t>Prevladujoča, značilna za tartufe</t>
   </si>
   <si>
-    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
-  </si>
-  <si>
-    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
-  </si>
-  <si>
     <t>Izdelek je v skladu z veljavno evropsko in nacionalno zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP.</t>
   </si>
   <si>
@@ -334,12 +349,15 @@
     <t>&lt;10</t>
   </si>
   <si>
+    <t>&lt;500</t>
+  </si>
+  <si>
+    <t>&lt;5.000</t>
+  </si>
+  <si>
     <t>&lt;100</t>
   </si>
   <si>
-    <t>&lt;500</t>
-  </si>
-  <si>
     <t>&lt;10.000</t>
   </si>
   <si>
@@ -355,13 +373,22 @@
     <t>1,3780</t>
   </si>
   <si>
+    <t>1,1427</t>
+  </si>
+  <si>
+    <t>1,3504</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,1893</t>
+  </si>
+  <si>
+    <t>1,4055</t>
+  </si>
+  <si>
     <t>75,0</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,1893</t>
-  </si>
-  <si>
-    <t>1,4055</t>
+    <t>74,0</t>
   </si>
   <si>
     <t xml:space="preserve"> 76,0</t>
@@ -373,52 +400,61 @@
     <t>8</t>
   </si>
   <si>
-    <t>1,1427</t>
-  </si>
-  <si>
-    <t>1,3504</t>
-  </si>
-  <si>
-    <t>74,0</t>
-  </si>
-  <si>
     <t>0,8</t>
   </si>
   <si>
+    <t>1422,1</t>
+  </si>
+  <si>
+    <t>1861</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
     <t>1429</t>
   </si>
   <si>
-    <t>1861</t>
-  </si>
-  <si>
-    <t>1523</t>
+    <t>334,7</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
+    <t>364</t>
   </si>
   <si>
     <t>336</t>
   </si>
   <si>
-    <t>445</t>
-  </si>
-  <si>
-    <t>364</t>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>16,6</t>
   </si>
   <si>
     <t>0,4</t>
   </si>
   <si>
-    <t>16,6</t>
+    <t>0,1</t>
   </si>
   <si>
     <t>3,6</t>
   </si>
   <si>
+    <t>80,7</t>
+  </si>
+  <si>
+    <t>63,5</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>83</t>
   </si>
   <si>
-    <t>63,5</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>61,1</t>
   </si>
   <si>
     <t>21,7</t>
@@ -427,102 +463,108 @@
     <t>0,6</t>
   </si>
   <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>8,1</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
     <t>0,2</t>
   </si>
   <si>
-    <t>8,1</t>
-  </si>
-  <si>
-    <t>72</t>
+    <t>0,0625</t>
   </si>
   <si>
     <t>0,018</t>
   </si>
   <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>7,7</t>
-  </si>
-  <si>
-    <t>2,7</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>32</t>
   </si>
   <si>
     <t>820</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>2,4</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>1875</t>
+    <t>225x150x85</t>
+  </si>
+  <si>
+    <t>110x400x190</t>
   </si>
   <si>
     <t>290x145x230</t>
   </si>
   <si>
+    <t>245x165x115</t>
+  </si>
+  <si>
     <t>192x138x87</t>
   </si>
   <si>
-    <t>110x400x190</t>
-  </si>
-  <si>
-    <t>245x165x115</t>
-  </si>
-  <si>
     <t>127x115x24</t>
   </si>
   <si>
+    <t>75x75x85</t>
+  </si>
+  <si>
     <t>57x57x131</t>
   </si>
   <si>
+    <t>110x40x190</t>
+  </si>
+  <si>
     <t>55x55x105</t>
   </si>
   <si>
+    <t>80x80x115</t>
+  </si>
+  <si>
     <t>62x65x85</t>
   </si>
   <si>
-    <t>110x40x190</t>
-  </si>
-  <si>
-    <t>80x80x115</t>
-  </si>
-  <si>
     <t>195x130x150</t>
   </si>
   <si>
     <t>V temnem in suhem prostoru pri temperaturi do 25 °C.</t>
   </si>
   <si>
+    <t>V temnem in suhem prostoru pri temperaturi 15-25 °C obrnjen s pokrovom navzgor.</t>
+  </si>
+  <si>
     <t>V temnem in suhem prostoru pri temperaturi 18-25 °C obrnjen s pokrovčkom navzgor.</t>
   </si>
   <si>
+    <t>V suhem prostoru.</t>
+  </si>
+  <si>
     <t>V temnem in suhem prostoru pri temperaturi 15-25 °C.</t>
   </si>
   <si>
     <t>V temnem, suhem prostoru pri sobni temperaturi obrnjen s pokrovom navzgor.</t>
   </si>
   <si>
-    <t>V suhem prostoru.</t>
-  </si>
-  <si>
     <t>Zaščiteno pred vlago in mehanskimi poškodbami. Tovor je potrebno zaščititi pred drsenjem, udarci in prevračanjem</t>
   </si>
   <si>
@@ -532,85 +574,97 @@
     <t>45 ml (5 x 9 ml)</t>
   </si>
   <si>
+    <t>250 g</t>
+  </si>
+  <si>
     <t>200 ml</t>
   </si>
   <si>
     <t>150 g</t>
   </si>
   <si>
-    <t>250 g</t>
-  </si>
-  <si>
     <t>24 mesecev</t>
   </si>
   <si>
+    <t>15 mesecev</t>
+  </si>
+  <si>
     <t>18 mesecev</t>
   </si>
   <si>
-    <t>15 mesecev</t>
-  </si>
-  <si>
     <t>36 mesecev</t>
   </si>
   <si>
+    <t>3 MPE ovitih v prozorno folijo</t>
+  </si>
+  <si>
     <t>6 MPE ovitih v prozorno folijo</t>
   </si>
   <si>
+    <t>Kartonska škatla</t>
+  </si>
+  <si>
     <t>6 MPE kartonasti zbirni zloženki</t>
   </si>
   <si>
     <t>6 MPE v kartonskem podstavku povitih s folijo</t>
   </si>
   <si>
-    <t>Kartonska škatla</t>
-  </si>
-  <si>
     <t>5 steklenih fiol s PP pokrovčki v plastičnem vložku in kartonski zloženki</t>
   </si>
   <si>
+    <t>Steklen kozarček s kovinskim pokrovčkom v kartonski zloženki</t>
+  </si>
+  <si>
     <t>temna steklenička s pokrovčkom v kartonski zloženki</t>
   </si>
   <si>
+    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
+  </si>
+  <si>
     <t>Vrečke z zip zapiranjem</t>
   </si>
   <si>
+    <t>pločevinka</t>
+  </si>
+  <si>
     <t>Steklen kozarec s kovinskim pokrovčkom</t>
   </si>
   <si>
-    <t>Kartonska škatla z 8 X 2 keksa zavita v foliji</t>
-  </si>
-  <si>
-    <t>pločevinka</t>
-  </si>
-  <si>
     <t>1800</t>
   </si>
   <si>
+    <t>1260</t>
+  </si>
+  <si>
     <t>1188</t>
   </si>
   <si>
+    <t>1920</t>
+  </si>
+  <si>
     <t>600</t>
   </si>
   <si>
+    <t>1008</t>
+  </si>
+  <si>
     <t>1392</t>
   </si>
   <si>
-    <t>1920</t>
-  </si>
-  <si>
-    <t>1008</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>16</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1025,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BL7"/>
+  <dimension ref="A1:BL8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -980,7 +1034,7 @@
     <col min="1" max="64" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64">
+    <row r="1" spans="1:63">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1170,602 +1224,700 @@
       <c r="BK1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:63">
+      <c r="A2" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:64">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="BA2" s="1" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>175</v>
+        <v>77</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>76</v>
+        <v>198</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>183</v>
+        <v>77</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:64">
+    <row r="3" spans="1:63">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>158</v>
+        <v>77</v>
       </c>
       <c r="BC3" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="BD3" s="1" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="BF3" s="1" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="BG3" s="1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="BH3" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="BI3" s="1" t="s">
-        <v>184</v>
+        <v>77</v>
       </c>
       <c r="BJ3" s="1" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="BK3" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="BL3" s="1" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:64">
+    <row r="4" spans="1:63">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="BC4" s="1" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="BE4" s="1" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="BF4" s="1" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="BG4" s="1" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="BH4" s="1" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="BI4" s="1" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="BJ4" s="1" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
       <c r="BK4" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="BL4" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:64">
+    <row r="5" spans="1:63">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="AQ5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS5" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="AZ5" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="BA5" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="BB5" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="BC5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="BD5" s="1" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="BE5" s="1" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="BF5" s="1" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="BG5" s="1" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="BH5" s="1" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="BI5" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="BJ5" s="1" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="BK5" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="BL5" s="1" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:64">
+    <row r="6" spans="1:63">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AR6" s="1" t="s">
-        <v>142</v>
+        <v>103</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="BA6" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
       <c r="BC6" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="BD6" s="1" t="s">
-        <v>168</v>
+        <v>184</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="BF6" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="BG6" s="1" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="BH6" s="1" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="BI6" s="1" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="BJ6" s="1" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="BK6" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="BL6" s="1" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:64">
+    <row r="7" spans="1:63">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="BA7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="BB7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BG7" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BK7" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63">
+      <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="W7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AC7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AO7" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="AM8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AQ7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AR7" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AW7" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AY7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AZ7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="BA7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BB7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="BC7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BD7" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="BE7" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="BF7" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="BG7" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="BH7" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="BI7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="BJ7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BK7" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="BL7" s="1" t="s">
-        <v>118</v>
+      <c r="AN8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AZ8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BC8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="BD8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="BE8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="BF8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BG8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BI8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BJ8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="BK8" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>